<commit_message>
- Geração dos valores boletos pagos, gerados e cartão - Colocando esses dados na planilha
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfdonadeli/Sites/metricas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfdonadeli/Sites/metricas/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -27,19 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
-  <si>
-    <t>Moeda:</t>
-  </si>
-  <si>
-    <t>Saldo:</t>
-  </si>
-  <si>
-    <t>Total Gasto:</t>
-  </si>
-  <si>
-    <t>Cartão:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Dia:</t>
   </si>
@@ -83,15 +71,6 @@
     <t>#Boletos Pagos:</t>
   </si>
   <si>
-    <t>%Conv. Boletos:</t>
-  </si>
-  <si>
-    <t>$CPV Efetivo:</t>
-  </si>
-  <si>
-    <t>$CPV Gerada:</t>
-  </si>
-  <si>
     <t>$Faturamento Cartão:</t>
   </si>
   <si>
@@ -107,18 +86,9 @@
     <t>%ROI:</t>
   </si>
   <si>
-    <t>#View/Impressões:</t>
-  </si>
-  <si>
-    <t>#View/Checkout:</t>
-  </si>
-  <si>
     <t>%Checkout/View:</t>
   </si>
   <si>
-    <t>#View/Purchase:</t>
-  </si>
-  <si>
     <t>%Purchase/View:</t>
   </si>
   <si>
@@ -152,18 +122,39 @@
     <t>#offsite_conversion</t>
   </si>
   <si>
-    <t>#end_of_file</t>
+    <t>$CPV:</t>
+  </si>
+  <si>
+    <t>#cartoes</t>
+  </si>
+  <si>
+    <t>#boletos_gerados</t>
+  </si>
+  <si>
+    <t>#boletos_pagos</t>
+  </si>
+  <si>
+    <t>#faturamento_boleto</t>
+  </si>
+  <si>
+    <t>#faturamento_cartao</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -172,12 +163,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB8CCE4"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -215,8 +200,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -225,45 +216,177 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -288,6 +411,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -580,265 +706,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="1" t="str">
+        <f>TEXT(VALUE($C2),"ddd")</f>
+        <v>Sat</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="str">
-        <f>TEXT(VALUE(C6),"ddd")</f>
-        <v>Sat</v>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="20" t="str">
+        <f>IFERROR($B5/($B12+$B15),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="34" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
+      <c r="B20" s="20" t="e">
+        <f>$B18+$B19</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
+      <c r="B21" s="20" t="str">
+        <f>IFERROR($B20-$B5,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="e">
-        <f>B18/B17</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="B22" s="21" t="str">
+        <f>IFERROR($B20/$B5,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6" t="e">
-        <f>B9/(B15+B17)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="B24" s="26"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="6" t="e">
-        <f>B9/(B16+B17)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+      <c r="B25" s="27"/>
+    </row>
+    <row r="26" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="6"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="6">
-        <f>B22+B23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="6" t="e">
-        <f>B24-B9</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="6" t="e">
-        <f>B24/B9</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" s="7"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="7"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="7"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="7"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="7"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>41</v>
-      </c>
+      <c r="B26" s="28"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B27" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+  <dataConsolidate/>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+  <conditionalFormatting sqref="B22">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Associacao dos postbacks com vendas (tela) - Readequacão do template colocando Geral no fim - Cálculo do Geral - Cálculo de métricas Views/Purchase/InitiateCheckout
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13280"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Dia:</t>
   </si>
@@ -125,26 +125,35 @@
     <t>$CPV:</t>
   </si>
   <si>
+    <t>#boletos_gerados</t>
+  </si>
+  <si>
+    <t>#boletos_pagos</t>
+  </si>
+  <si>
     <t>#cartoes</t>
   </si>
   <si>
-    <t>#boletos_gerados</t>
-  </si>
-  <si>
-    <t>#boletos_pagos</t>
-  </si>
-  <si>
     <t>#faturamento_boleto</t>
   </si>
   <si>
     <t>#faturamento_cartao</t>
+  </si>
+  <si>
+    <t>#checkout_view</t>
+  </si>
+  <si>
+    <t>#purchase_view</t>
+  </si>
+  <si>
+    <t>#purchase_checkout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -156,6 +165,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -207,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -216,43 +230,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
         <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
+      </left>
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top style="thin">
@@ -263,150 +244,34 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -709,227 +574,223 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="str">
+      <c r="B1" s="4" t="str">
         <f>TEXT(VALUE($C2),"ddd")</f>
         <v>Sat</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="17"/>
-    </row>
-    <row r="13" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="33" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="33" t="s">
-        <v>34</v>
-      </c>
-    </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="20" t="str">
+      <c r="B17" s="10" t="str">
         <f>IFERROR($B5/($B12+$B15),"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="24" t="s">
+      <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="20" t="e">
-        <f>$B18+$B19</f>
-        <v>#VALUE!</v>
+      <c r="B20" s="10" t="str">
+        <f>IFERROR(IF($B18+$B19&lt;&gt;0,$B18+$B19,0),"")</f>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="20" t="str">
+      <c r="B21" s="10" t="str">
         <f>IFERROR($B20-$B5,"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="21" t="str">
+      <c r="B22" s="11" t="str">
         <f>IFERROR($B20/$B5,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="26"/>
+      <c r="B24" s="15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="27"/>
-    </row>
-    <row r="26" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="B25" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="28"/>
+      <c r="B26" s="15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="5"/>
+      <c r="B27" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <dataConsolidate/>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="greaterThanOrEqual">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
- Testes de inserção de insights - Preparação da planilha com fórmulas do campo geral - Formatação condicional no campo ROI na planilha
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -571,13 +571,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -586,16 +586,16 @@
     <col min="2" max="3" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="str">
-        <f>TEXT(VALUE($C2),"ddd")</f>
-        <v>Sat</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="e">
+        <f>TEXT(VALUE($B2),"ddd")</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -603,7 +603,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -611,7 +611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -619,7 +619,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -627,7 +627,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -643,7 +643,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -651,7 +651,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
@@ -659,11 +659,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="G10" t="e">
+        <f>av</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
@@ -671,17 +675,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="7"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -689,7 +693,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
@@ -697,7 +701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
@@ -753,7 +757,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="11" t="str">
-        <f>IFERROR($B20/$B5,"")</f>
+        <f>IFERROR($B21/$B5,"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
- Template com fonte menor
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -163,12 +163,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -247,25 +247,22 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,145 +568,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="25.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.83203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="e">
+      <c r="B1" s="1" t="e">
         <f>TEXT(VALUE($B2),"ddd")</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="G10" t="e">
-        <f>av</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="G10" s="2" t="str">
+        <f>IFERROR(AVERAGE(A1:A2),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" s="10" t="s">
         <v>31</v>
       </c>
@@ -718,23 +716,23 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="10" t="s">
         <v>16</v>
       </c>
@@ -743,7 +741,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="10" t="s">
         <v>17</v>
       </c>
@@ -752,7 +750,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="10" t="s">
         <v>18</v>
       </c>
@@ -761,36 +759,33 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="3"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
- Alteração de Valor por para Custo por - Round para fórmulas
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -574,7 +574,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -712,7 +712,7 @@
         <v>31</v>
       </c>
       <c r="B17" s="10" t="str">
-        <f>IFERROR($B5/($B12+$B15),"")</f>
+        <f>IFERROR(ROUND($B5/($B12+$B15),2),"")</f>
         <v/>
       </c>
     </row>
@@ -755,7 +755,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="11" t="str">
-        <f>IFERROR($B21/$B5,"")</f>
+        <f>IFERROR(ROUND($B21/$B5,2),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
- Adicionando Template Visual - Foto do Perfil - Escondendo algumas informações no template Excel
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -574,7 +574,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -683,7 +683,7 @@
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -691,7 +691,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
@@ -716,7 +716,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.15">
       <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
@@ -724,7 +724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.15">
       <c r="A19" s="10" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
- Dia da semana no template, acerto - Inversão da lista de vendas na plataforma, por data decrescente - Lista de activities
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Dia:</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>#purchase_checkout</t>
+  </si>
+  <si>
+    <t>#dia_da_semana</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -588,9 +591,8 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="e">
-        <f>TEXT(VALUE($B2),"ddd")</f>
-        <v>#VALUE!</v>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
- Adicionando KPIs na planilha
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13280"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13280" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
+    <sheet name="KPI" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
   <si>
     <t>Dia:</t>
   </si>
@@ -150,13 +151,79 @@
   </si>
   <si>
     <t>#dia_da_semana</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>Cliques/Venda</t>
+  </si>
+  <si>
+    <t>CPV</t>
+  </si>
+  <si>
+    <t>CPC Máximo</t>
+  </si>
+  <si>
+    <t>Este Anúncio</t>
+  </si>
+  <si>
+    <t>Meta 1</t>
+  </si>
+  <si>
+    <t>Meta 2</t>
+  </si>
+  <si>
+    <t>Meta 3</t>
+  </si>
+  <si>
+    <t>LPV</t>
+  </si>
+  <si>
+    <t>% Cartões</t>
+  </si>
+  <si>
+    <t>% Boletos</t>
+  </si>
+  <si>
+    <t>Conversão Boletos</t>
+  </si>
+  <si>
+    <t>CTR</t>
+  </si>
+  <si>
+    <t>CPC</t>
+  </si>
+  <si>
+    <t>CPM</t>
+  </si>
+  <si>
+    <t>Este anúncio</t>
+  </si>
+  <si>
+    <t>Vitalício</t>
+  </si>
+  <si>
+    <t>Última semana</t>
+  </si>
+  <si>
+    <t>Últimos três dias</t>
+  </si>
+  <si>
+    <t>Meta 4</t>
+  </si>
+  <si>
+    <t>Taxa Conversao</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -172,6 +239,24 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="9">
@@ -224,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -247,12 +332,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -266,8 +405,34 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -573,11 +738,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -685,7 +850,7 @@
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -693,7 +858,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
@@ -701,7 +866,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
@@ -718,7 +883,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="10" t="s">
         <v>14</v>
       </c>
@@ -726,7 +891,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="10" t="s">
         <v>15</v>
       </c>
@@ -795,4 +960,1098 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:U23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="16"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="U3" s="13"/>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="27" t="e">
+        <f>(comissao/E4)-1</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D4" s="19" t="e">
+        <f>ViewContents/Vendas</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E4" s="19" t="e">
+        <f>F4*D4</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F4" s="19" t="e">
+        <f>AVERAGE(Métricas!Primeira7:Ultima7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="27" t="e">
+        <f>(comissao/L4)-1</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K4" s="19" t="e">
+        <f>IFERROR((SUM(ViewContents_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L4" s="19" t="e">
+        <f>M4*K4</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M4" s="19" t="e">
+        <f>AVERAGE(Métricas!Primeira7dias7:Ultima7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N4" s="14"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" s="28" t="e">
+        <f>(comissao/S4)-1</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R4" s="20" t="e">
+        <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S4" s="20" t="e">
+        <f>T4*R4</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T4" s="20" t="e">
+        <f>AVERAGE(Métricas!Primeira3dias7:Ultima7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U4" s="13"/>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="19" t="e">
+        <f>ViewContents/Vendas</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E5" s="19" t="e">
+        <f>comissao/(1+C5)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F5" s="19" t="e">
+        <f>E5/D5</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="19" t="e">
+        <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L5" s="19" t="e">
+        <f>comissao/(1+J5)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M5" s="19" t="e">
+        <f>L5/K5</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N5" s="14"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="20" t="e">
+        <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S5" s="20" t="e">
+        <f>comissao/(Q5+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T5" s="20" t="e">
+        <f>S5/R5</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U5" s="13"/>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B6" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="19" t="e">
+        <f>ViewContents/Vendas</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E6" s="19" t="e">
+        <f>comissao/(1+C6)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F6" s="19" t="e">
+        <f t="shared" ref="F6:F8" si="0">E6/D6</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="K6" s="19" t="e">
+        <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L6" s="19" t="e">
+        <f>comissao/(1+J6)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M6" s="19" t="e">
+        <f t="shared" ref="M6:M8" si="1">L6/K6</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N6" s="14"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>0.8</v>
+      </c>
+      <c r="R6" s="20" t="e">
+        <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S6" s="20" t="e">
+        <f>comissao/(Q6+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T6" s="20" t="e">
+        <f t="shared" ref="T6:T8" si="2">S6/R6</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="21">
+        <v>1</v>
+      </c>
+      <c r="D7" s="19" t="e">
+        <f>ViewContents/Vendas</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E7" s="19" t="e">
+        <f>comissao/(1+C7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F7" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="21">
+        <v>1</v>
+      </c>
+      <c r="K7" s="19" t="e">
+        <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L7" s="19" t="e">
+        <f>comissao/(1+J7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M7" s="19" t="e">
+        <f t="shared" si="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="N7" s="14"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q7" s="21">
+        <v>1</v>
+      </c>
+      <c r="R7" s="20" t="e">
+        <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S7" s="20" t="e">
+        <f>comissao/(Q7+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T7" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="U7" s="13"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B8" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="D8" s="19" t="e">
+        <f>ViewContents/Vendas</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E8" s="19" t="e">
+        <f>comissao/(1+C8)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F8" s="19" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="K8" s="19" t="e">
+        <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L8" s="19" t="e">
+        <f>comissao/(1+J8)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M8" s="19" t="e">
+        <f t="shared" si="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="N8" s="14"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q8" s="21">
+        <v>1.2</v>
+      </c>
+      <c r="R8" s="20" t="e">
+        <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S8" s="20" t="e">
+        <f>comissao/(Q8+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T8" s="20" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="U8" s="13"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B11" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="22" t="e">
+        <f>Métricas!Geral5/Vendas</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="22" t="e">
+        <f>IFERROR(SUM(Métricas!Primeira7dias5:Ultima5)/Venda_7dias,C11)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q11" s="22" t="e">
+        <f>IFERROR(SUM(Métricas!Primeira3dias5:Ultima5)/Venda_3dias,C11)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B12" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="29" t="e">
+        <f>Cartoes/Vendas</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="29">
+        <f>IFERROR(Cartao_7dias/Venda_7dias,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q12" s="29">
+        <f>IFERROR(Cartao_3dias/Venda_3dias,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B13" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="29" t="e">
+        <f>BoletosPagos/Vendas</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="29">
+        <f>IFERROR(BoletosPago_7dias/Venda_7dias,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13" s="29">
+        <f>IFERROR(BoletosPago_3dias/Venda_3dias,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B14" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="29" t="e">
+        <f>BoletosPagos/BoletosTotais</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J14" s="29" t="e">
+        <f>IFERROR(Boletos_Pago_7dias/BoletosTotal_7dias,C14)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q14" s="29" t="e">
+        <f>IFERROR(Boletos_Pago_3dias/BoletosTotal_3dias,C14)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B15" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="30" t="e">
+        <f>((1/D4)*C12)+((1/D4)*C13*C14)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="30" t="e">
+        <f>IF(IFERROR(((1/K4)*J12)+((1/K4)*J13*J14),C15)=0,C15,IFERROR(((1/K4)*J12)+((1/K4)*J13*J14),C15))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q15" s="30" t="e">
+        <f>IF(IFERROR(((1/R4)*Q12)+((1/R4)*Q13*Q14),C15)=0,C15,IFERROR(((1/R4)*Q12)+((1/R4)*Q13*Q14),C15))</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B16" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="29" t="e">
+        <f>AVERAGE(Métricas!Primeira6:Ultima6)/100</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J16" s="29" t="e">
+        <f>AVERAGE(Métricas!Primeira7dias6:Ultima6)/100</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q16" s="29" t="e">
+        <f>AVERAGE(Métricas!Primeira3dias6:Ultima6)/100</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B18" s="13"/>
+      <c r="C18" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="22" t="e">
+        <f>(30/C11)-1</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D19" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="E19" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="F19" s="24">
+        <v>1</v>
+      </c>
+      <c r="G19" s="24">
+        <v>1.2</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="22">
+        <f>IFERROR((comissao/J11)-1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="24">
+        <v>0.5</v>
+      </c>
+      <c r="L19" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="M19" s="24">
+        <v>1</v>
+      </c>
+      <c r="N19" s="24">
+        <v>1.2</v>
+      </c>
+      <c r="O19" s="13"/>
+      <c r="P19" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q19" s="25">
+        <f>IFERROR((comissao/Q11)-1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="S19" s="26">
+        <v>0.8</v>
+      </c>
+      <c r="T19" s="26">
+        <v>1</v>
+      </c>
+      <c r="U19" s="26">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="22" t="e">
+        <f>C11</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D20" s="22" t="e">
+        <f>comissao/(D19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E20" s="22" t="e">
+        <f>comissao/(E19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F20" s="22" t="e">
+        <f>comissao/(F19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G20" s="22" t="e">
+        <f>comissao/(G19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="J20" s="22" t="e">
+        <f>J11</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K20" s="22" t="e">
+        <f>comissao/(K19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L20" s="22" t="e">
+        <f>comissao/(L19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M20" s="22" t="e">
+        <f>comissao/(M19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N20" s="22" t="e">
+        <f>comissao/(N19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O20" s="13"/>
+      <c r="P20" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q20" s="25" t="e">
+        <f>Q11</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R20" s="25" t="e">
+        <f>comissao/(R19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S20" s="25" t="e">
+        <f>comissao/(S19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T20" s="25" t="e">
+        <f>comissao/(T19+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U20" s="25" t="e">
+        <f>comissao/(U19+1)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B21" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="22" t="e">
+        <f>1/C15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D21" s="22" t="e">
+        <f>1/C15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E21" s="22" t="e">
+        <f>1/C15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F21" s="22" t="e">
+        <f>1/C15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G21" s="22" t="e">
+        <f>1/C15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H21" s="13"/>
+      <c r="I21" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="J21" s="22" t="e">
+        <f>1/J15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K21" s="22" t="e">
+        <f>1/J15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L21" s="22" t="e">
+        <f>1/J15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M21" s="22" t="e">
+        <f>1/J15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N21" s="22" t="e">
+        <f>1/J15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O21" s="13"/>
+      <c r="P21" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q21" s="25" t="e">
+        <f>1/Q15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R21" s="25" t="e">
+        <f>1/Q15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S21" s="25" t="e">
+        <f>1/Q15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T21" s="25" t="e">
+        <f>1/Q15</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U21" s="25" t="e">
+        <f>1/Q15</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B22" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="22" t="e">
+        <f>C20/C21</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D22" s="22" t="e">
+        <f>D20/D21</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E22" s="22" t="e">
+        <f>E20/E21</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F22" s="22" t="e">
+        <f>F20/F21</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G22" s="22" t="e">
+        <f>G20/G21</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H22" s="13"/>
+      <c r="I22" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="J22" s="22" t="e">
+        <f>J20/J21</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K22" s="22" t="e">
+        <f t="shared" ref="K22:N22" si="3">K20/K21</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L22" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="M22" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="N22" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="O22" s="13"/>
+      <c r="P22" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q22" s="25" t="e">
+        <f>Q20/Q21</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R22" s="25" t="e">
+        <f t="shared" ref="R22:U22" si="4">R20/R21</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S22" s="25" t="e">
+        <f t="shared" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="T22" s="25" t="e">
+        <f t="shared" si="4"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="U22" s="25" t="e">
+        <f t="shared" si="4"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B23" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="22" t="e">
+        <f>(1/C16)*C22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D23" s="22" t="e">
+        <f>(1/C16)*D22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E23" s="22" t="e">
+        <f>(1/C16)*E22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F23" s="22" t="e">
+        <f>(1/C16)*F22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G23" s="22" t="e">
+        <f>(1/C16)*G22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H23" s="13"/>
+      <c r="I23" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="22" t="e">
+        <f>(1/J16)*J22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K23" s="22" t="e">
+        <f>(1/J16)*K22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L23" s="22" t="e">
+        <f>(1/J16)*L22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M23" s="22" t="e">
+        <f>(1/J16)*M22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N23" s="22" t="e">
+        <f>(1/J16)*N22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O23" s="13"/>
+      <c r="P23" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q23" s="25" t="e">
+        <f>(1/Q16)*Q22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R23" s="25" t="e">
+        <f>(1/Q16)*R22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S23" s="25" t="e">
+        <f>(1/Q16)*S22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T23" s="25" t="e">
+        <f>(1/Q16)*T22</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U23" s="25" t="e">
+        <f>(1/Q16/100)*U22</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Ajeitando KPIs no template
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="13280" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -417,18 +417,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -967,7 +973,7 @@
   <dimension ref="B1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1078,19 +1084,19 @@
       <c r="B4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="27" t="e">
+      <c r="C4" s="24" t="e">
         <f>(comissao/E4)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="D4" s="19" t="e">
-        <f>ViewContents/Vendas</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E4" s="19" t="e">
+      <c r="D4" s="34" t="e">
+        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E4" s="28" t="e">
         <f>F4*D4</f>
         <v>#NAME?</v>
       </c>
-      <c r="F4" s="19" t="e">
+      <c r="F4" s="28" t="e">
         <f>AVERAGE(Métricas!Primeira7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
@@ -1099,19 +1105,19 @@
       <c r="I4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="27" t="e">
+      <c r="J4" s="24" t="e">
         <f>(comissao/L4)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="K4" s="19" t="e">
-        <f>IFERROR((SUM(ViewContents_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L4" s="19" t="e">
+      <c r="K4" s="34" t="e">
+        <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L4" s="28" t="e">
         <f>M4*K4</f>
         <v>#NAME?</v>
       </c>
-      <c r="M4" s="19" t="e">
+      <c r="M4" s="28" t="e">
         <f>AVERAGE(Métricas!Primeira7dias7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
@@ -1120,19 +1126,19 @@
       <c r="P4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" s="28" t="e">
+      <c r="Q4" s="25" t="e">
         <f>(comissao/S4)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="R4" s="20" t="e">
+      <c r="R4" s="35" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S4" s="20" t="e">
+      <c r="S4" s="30" t="e">
         <f>T4*R4</f>
         <v>#NAME?</v>
       </c>
-      <c r="T4" s="20" t="e">
+      <c r="T4" s="30" t="e">
         <f>AVERAGE(Métricas!Primeira3dias7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
@@ -1142,18 +1148,18 @@
       <c r="B5" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="19">
         <v>0.5</v>
       </c>
-      <c r="D5" s="19" t="e">
-        <f>ViewContents/Vendas</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E5" s="19" t="e">
+      <c r="D5" s="34" t="e">
+        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E5" s="28" t="e">
         <f>comissao/(1+C5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F5" s="19" t="e">
+      <c r="F5" s="28" t="e">
         <f>E5/D5</f>
         <v>#NAME?</v>
       </c>
@@ -1162,18 +1168,18 @@
       <c r="I5" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="19">
         <v>0.5</v>
       </c>
-      <c r="K5" s="19" t="e">
+      <c r="K5" s="34" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L5" s="19" t="e">
+      <c r="L5" s="28" t="e">
         <f>comissao/(1+J5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M5" s="19" t="e">
+      <c r="M5" s="28" t="e">
         <f>L5/K5</f>
         <v>#NAME?</v>
       </c>
@@ -1182,18 +1188,18 @@
       <c r="P5" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="Q5" s="21">
+      <c r="Q5" s="19">
         <v>0.5</v>
       </c>
-      <c r="R5" s="20" t="e">
+      <c r="R5" s="35" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S5" s="20" t="e">
+      <c r="S5" s="30" t="e">
         <f>comissao/(Q5+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T5" s="20" t="e">
+      <c r="T5" s="30" t="e">
         <f>S5/R5</f>
         <v>#NAME?</v>
       </c>
@@ -1203,18 +1209,18 @@
       <c r="B6" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="19">
         <v>0.8</v>
       </c>
-      <c r="D6" s="19" t="e">
-        <f>ViewContents/Vendas</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E6" s="19" t="e">
+      <c r="D6" s="34" t="e">
+        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E6" s="28" t="e">
         <f>comissao/(1+C6)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F6" s="19" t="e">
+      <c r="F6" s="28" t="e">
         <f t="shared" ref="F6:F8" si="0">E6/D6</f>
         <v>#NAME?</v>
       </c>
@@ -1223,18 +1229,18 @@
       <c r="I6" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="21">
+      <c r="J6" s="19">
         <v>0.8</v>
       </c>
-      <c r="K6" s="19" t="e">
+      <c r="K6" s="34" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L6" s="19" t="e">
+      <c r="L6" s="28" t="e">
         <f>comissao/(1+J6)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M6" s="19" t="e">
+      <c r="M6" s="28" t="e">
         <f t="shared" ref="M6:M8" si="1">L6/K6</f>
         <v>#NAME?</v>
       </c>
@@ -1243,18 +1249,18 @@
       <c r="P6" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="Q6" s="21">
+      <c r="Q6" s="19">
         <v>0.8</v>
       </c>
-      <c r="R6" s="20" t="e">
+      <c r="R6" s="35" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S6" s="20" t="e">
+      <c r="S6" s="30" t="e">
         <f>comissao/(Q6+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T6" s="20" t="e">
+      <c r="T6" s="30" t="e">
         <f t="shared" ref="T6:T8" si="2">S6/R6</f>
         <v>#NAME?</v>
       </c>
@@ -1264,18 +1270,18 @@
       <c r="B7" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="19">
         <v>1</v>
       </c>
-      <c r="D7" s="19" t="e">
-        <f>ViewContents/Vendas</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E7" s="19" t="e">
+      <c r="D7" s="34" t="e">
+        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E7" s="28" t="e">
         <f>comissao/(1+C7)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F7" s="19" t="e">
+      <c r="F7" s="28" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
@@ -1284,18 +1290,18 @@
       <c r="I7" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="19">
         <v>1</v>
       </c>
-      <c r="K7" s="19" t="e">
+      <c r="K7" s="34" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L7" s="19" t="e">
+      <c r="L7" s="28" t="e">
         <f>comissao/(1+J7)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M7" s="19" t="e">
+      <c r="M7" s="28" t="e">
         <f t="shared" si="1"/>
         <v>#NAME?</v>
       </c>
@@ -1304,18 +1310,18 @@
       <c r="P7" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="Q7" s="21">
+      <c r="Q7" s="19">
         <v>1</v>
       </c>
-      <c r="R7" s="20" t="e">
+      <c r="R7" s="35" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S7" s="20" t="e">
+      <c r="S7" s="30" t="e">
         <f>comissao/(Q7+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T7" s="20" t="e">
+      <c r="T7" s="30" t="e">
         <f t="shared" si="2"/>
         <v>#NAME?</v>
       </c>
@@ -1325,18 +1331,18 @@
       <c r="B8" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="19">
         <v>1.2</v>
       </c>
-      <c r="D8" s="19" t="e">
-        <f>ViewContents/Vendas</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E8" s="19" t="e">
+      <c r="D8" s="34" t="e">
+        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E8" s="28" t="e">
         <f>comissao/(1+C8)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F8" s="19" t="e">
+      <c r="F8" s="28" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
@@ -1345,18 +1351,18 @@
       <c r="I8" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="21">
+      <c r="J8" s="19">
         <v>1.2</v>
       </c>
-      <c r="K8" s="19" t="e">
+      <c r="K8" s="34" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L8" s="19" t="e">
+      <c r="L8" s="28" t="e">
         <f>comissao/(1+J8)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M8" s="19" t="e">
+      <c r="M8" s="28" t="e">
         <f t="shared" si="1"/>
         <v>#NAME?</v>
       </c>
@@ -1365,18 +1371,18 @@
       <c r="P8" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="Q8" s="21">
+      <c r="Q8" s="19">
         <v>1.2</v>
       </c>
-      <c r="R8" s="20" t="e">
+      <c r="R8" s="35" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S8" s="20" t="e">
+      <c r="S8" s="30" t="e">
         <f>comissao/(Q8+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T8" s="20" t="e">
+      <c r="T8" s="30" t="e">
         <f t="shared" si="2"/>
         <v>#NAME?</v>
       </c>
@@ -1430,8 +1436,8 @@
       <c r="B11" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="22" t="e">
-        <f>Métricas!Geral5/Vendas</f>
+      <c r="C11" s="29" t="e">
+        <f>IF(Vendas = 0, E4, Métricas!Geral5/Vendas)</f>
         <v>#NAME?</v>
       </c>
       <c r="D11" s="13"/>
@@ -1442,7 +1448,7 @@
       <c r="I11" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="22" t="e">
+      <c r="J11" s="29" t="e">
         <f>IFERROR(SUM(Métricas!Primeira7dias5:Ultima5)/Venda_7dias,C11)</f>
         <v>#NAME?</v>
       </c>
@@ -1454,7 +1460,7 @@
       <c r="P11" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="Q11" s="22" t="e">
+      <c r="Q11" s="29" t="e">
         <f>IFERROR(SUM(Métricas!Primeira3dias5:Ultima5)/Venda_3dias,C11)</f>
         <v>#NAME?</v>
       </c>
@@ -1467,7 +1473,7 @@
       <c r="B12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="29" t="e">
+      <c r="C12" s="26" t="e">
         <f>Cartoes/Vendas</f>
         <v>#NAME?</v>
       </c>
@@ -1479,7 +1485,7 @@
       <c r="I12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="29">
+      <c r="J12" s="26">
         <f>IFERROR(Cartao_7dias/Venda_7dias,0)</f>
         <v>0</v>
       </c>
@@ -1488,10 +1494,10 @@
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
-      <c r="P12" s="23" t="s">
+      <c r="P12" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="Q12" s="29">
+      <c r="Q12" s="26">
         <f>IFERROR(Cartao_3dias/Venda_3dias,0)</f>
         <v>0</v>
       </c>
@@ -1504,7 +1510,7 @@
       <c r="B13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="29" t="e">
+      <c r="C13" s="26" t="e">
         <f>BoletosPagos/Vendas</f>
         <v>#NAME?</v>
       </c>
@@ -1516,7 +1522,7 @@
       <c r="I13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="J13" s="29">
+      <c r="J13" s="26">
         <f>IFERROR(BoletosPago_7dias/Venda_7dias,0)</f>
         <v>0</v>
       </c>
@@ -1525,10 +1531,10 @@
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
-      <c r="P13" s="23" t="s">
+      <c r="P13" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q13" s="29">
+      <c r="Q13" s="26">
         <f>IFERROR(BoletosPago_3dias/Venda_3dias,0)</f>
         <v>0</v>
       </c>
@@ -1541,7 +1547,7 @@
       <c r="B14" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="29" t="e">
+      <c r="C14" s="26" t="e">
         <f>BoletosPagos/BoletosTotais</f>
         <v>#NAME?</v>
       </c>
@@ -1553,7 +1559,7 @@
       <c r="I14" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="29" t="e">
+      <c r="J14" s="26" t="e">
         <f>IFERROR(Boletos_Pago_7dias/BoletosTotal_7dias,C14)</f>
         <v>#NAME?</v>
       </c>
@@ -1562,10 +1568,10 @@
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
-      <c r="P14" s="23" t="s">
+      <c r="P14" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="Q14" s="29" t="e">
+      <c r="Q14" s="26" t="e">
         <f>IFERROR(Boletos_Pago_3dias/BoletosTotal_3dias,C14)</f>
         <v>#NAME?</v>
       </c>
@@ -1578,7 +1584,7 @@
       <c r="B15" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="30" t="e">
+      <c r="C15" s="27" t="e">
         <f>((1/D4)*C12)+((1/D4)*C13*C14)</f>
         <v>#NAME?</v>
       </c>
@@ -1590,7 +1596,7 @@
       <c r="I15" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="J15" s="30" t="e">
+      <c r="J15" s="27" t="e">
         <f>IF(IFERROR(((1/K4)*J12)+((1/K4)*J13*J14),C15)=0,C15,IFERROR(((1/K4)*J12)+((1/K4)*J13*J14),C15))</f>
         <v>#NAME?</v>
       </c>
@@ -1602,7 +1608,7 @@
       <c r="P15" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="Q15" s="30" t="e">
+      <c r="Q15" s="27" t="e">
         <f>IF(IFERROR(((1/R4)*Q12)+((1/R4)*Q13*Q14),C15)=0,C15,IFERROR(((1/R4)*Q12)+((1/R4)*Q13*Q14),C15))</f>
         <v>#NAME?</v>
       </c>
@@ -1615,7 +1621,7 @@
       <c r="B16" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="29" t="e">
+      <c r="C16" s="26" t="e">
         <f>AVERAGE(Métricas!Primeira6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
@@ -1627,7 +1633,7 @@
       <c r="I16" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="J16" s="29" t="e">
+      <c r="J16" s="26" t="e">
         <f>AVERAGE(Métricas!Primeira7dias6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
@@ -1636,10 +1642,10 @@
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
-      <c r="P16" s="23" t="s">
+      <c r="P16" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="Q16" s="29" t="e">
+      <c r="Q16" s="26" t="e">
         <f>AVERAGE(Métricas!Primeira3dias6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
@@ -1672,7 +1678,7 @@
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B18" s="13"/>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="20" t="s">
         <v>56</v>
       </c>
       <c r="D18" s="13"/>
@@ -1681,7 +1687,7 @@
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
-      <c r="J18" s="22" t="s">
+      <c r="J18" s="20" t="s">
         <v>56</v>
       </c>
       <c r="K18" s="13"/>
@@ -1690,7 +1696,7 @@
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
-      <c r="Q18" s="22" t="s">
+      <c r="Q18" s="20" t="s">
         <v>56</v>
       </c>
       <c r="R18" s="13"/>
@@ -1702,60 +1708,60 @@
       <c r="B19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="22" t="e">
+      <c r="C19" s="26" t="e">
         <f>(30/C11)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="22">
         <v>0.5</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="22">
         <v>0.8</v>
       </c>
-      <c r="F19" s="24">
+      <c r="F19" s="22">
         <v>1</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="22">
         <v>1.2</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="26">
         <f>IFERROR((comissao/J11)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="22">
         <v>0.5</v>
       </c>
-      <c r="L19" s="24">
+      <c r="L19" s="22">
         <v>0.8</v>
       </c>
-      <c r="M19" s="24">
+      <c r="M19" s="22">
         <v>1</v>
       </c>
-      <c r="N19" s="24">
+      <c r="N19" s="22">
         <v>1.2</v>
       </c>
       <c r="O19" s="13"/>
       <c r="P19" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="Q19" s="25">
+      <c r="Q19" s="36">
         <f>IFERROR((comissao/Q11)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="R19" s="26">
+      <c r="R19" s="23">
         <v>0.5</v>
       </c>
-      <c r="S19" s="26">
+      <c r="S19" s="23">
         <v>0.8</v>
       </c>
-      <c r="T19" s="26">
+      <c r="T19" s="23">
         <v>1</v>
       </c>
-      <c r="U19" s="26">
+      <c r="U19" s="23">
         <v>1.2</v>
       </c>
     </row>
@@ -1763,23 +1769,23 @@
       <c r="B20" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="22" t="e">
+      <c r="C20" s="29" t="e">
         <f>C11</f>
         <v>#NAME?</v>
       </c>
-      <c r="D20" s="22" t="e">
+      <c r="D20" s="29" t="e">
         <f>comissao/(D19+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E20" s="22" t="e">
+      <c r="E20" s="29" t="e">
         <f>comissao/(E19+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F20" s="22" t="e">
+      <c r="F20" s="29" t="e">
         <f>comissao/(F19+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="G20" s="22" t="e">
+      <c r="G20" s="29" t="e">
         <f>comissao/(G19+1)</f>
         <v>#NAME?</v>
       </c>
@@ -1787,47 +1793,47 @@
       <c r="I20" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="22" t="e">
+      <c r="J20" s="29" t="e">
         <f>J11</f>
         <v>#NAME?</v>
       </c>
-      <c r="K20" s="22" t="e">
+      <c r="K20" s="29" t="e">
         <f>comissao/(K19+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L20" s="22" t="e">
+      <c r="L20" s="29" t="e">
         <f>comissao/(L19+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M20" s="22" t="e">
+      <c r="M20" s="29" t="e">
         <f>comissao/(M19+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N20" s="22" t="e">
+      <c r="N20" s="29" t="e">
         <f>comissao/(N19+1)</f>
         <v>#NAME?</v>
       </c>
       <c r="O20" s="13"/>
-      <c r="P20" s="23" t="s">
+      <c r="P20" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="Q20" s="25" t="e">
+      <c r="Q20" s="31" t="e">
         <f>Q11</f>
         <v>#NAME?</v>
       </c>
-      <c r="R20" s="25" t="e">
+      <c r="R20" s="31" t="e">
         <f>comissao/(R19+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S20" s="25" t="e">
+      <c r="S20" s="31" t="e">
         <f>comissao/(S19+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T20" s="25" t="e">
+      <c r="T20" s="31" t="e">
         <f>comissao/(T19+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="U20" s="25" t="e">
+      <c r="U20" s="31" t="e">
         <f>comissao/(U19+1)</f>
         <v>#NAME?</v>
       </c>
@@ -1836,23 +1842,23 @@
       <c r="B21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="22" t="e">
+      <c r="C21" s="33" t="e">
         <f>1/C15</f>
         <v>#NAME?</v>
       </c>
-      <c r="D21" s="22" t="e">
+      <c r="D21" s="33" t="e">
         <f>1/C15</f>
         <v>#NAME?</v>
       </c>
-      <c r="E21" s="22" t="e">
+      <c r="E21" s="33" t="e">
         <f>1/C15</f>
         <v>#NAME?</v>
       </c>
-      <c r="F21" s="22" t="e">
+      <c r="F21" s="33" t="e">
         <f>1/C15</f>
         <v>#NAME?</v>
       </c>
-      <c r="G21" s="22" t="e">
+      <c r="G21" s="33" t="e">
         <f>1/C15</f>
         <v>#NAME?</v>
       </c>
@@ -1860,47 +1866,47 @@
       <c r="I21" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J21" s="22" t="e">
+      <c r="J21" s="33" t="e">
         <f>1/J15</f>
         <v>#NAME?</v>
       </c>
-      <c r="K21" s="22" t="e">
+      <c r="K21" s="33" t="e">
         <f>1/J15</f>
         <v>#NAME?</v>
       </c>
-      <c r="L21" s="22" t="e">
+      <c r="L21" s="33" t="e">
         <f>1/J15</f>
         <v>#NAME?</v>
       </c>
-      <c r="M21" s="22" t="e">
+      <c r="M21" s="33" t="e">
         <f>1/J15</f>
         <v>#NAME?</v>
       </c>
-      <c r="N21" s="22" t="e">
+      <c r="N21" s="33" t="e">
         <f>1/J15</f>
         <v>#NAME?</v>
       </c>
       <c r="O21" s="13"/>
-      <c r="P21" s="23" t="s">
+      <c r="P21" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="Q21" s="25" t="e">
+      <c r="Q21" s="32" t="e">
         <f>1/Q15</f>
         <v>#NAME?</v>
       </c>
-      <c r="R21" s="25" t="e">
+      <c r="R21" s="32" t="e">
         <f>1/Q15</f>
         <v>#NAME?</v>
       </c>
-      <c r="S21" s="25" t="e">
+      <c r="S21" s="32" t="e">
         <f>1/Q15</f>
         <v>#NAME?</v>
       </c>
-      <c r="T21" s="25" t="e">
+      <c r="T21" s="32" t="e">
         <f>1/Q15</f>
         <v>#NAME?</v>
       </c>
-      <c r="U21" s="25" t="e">
+      <c r="U21" s="32" t="e">
         <f>1/Q15</f>
         <v>#NAME?</v>
       </c>
@@ -1909,23 +1915,23 @@
       <c r="B22" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="22" t="e">
+      <c r="C22" s="29" t="e">
         <f>C20/C21</f>
         <v>#NAME?</v>
       </c>
-      <c r="D22" s="22" t="e">
+      <c r="D22" s="29" t="e">
         <f>D20/D21</f>
         <v>#NAME?</v>
       </c>
-      <c r="E22" s="22" t="e">
+      <c r="E22" s="29" t="e">
         <f>E20/E21</f>
         <v>#NAME?</v>
       </c>
-      <c r="F22" s="22" t="e">
+      <c r="F22" s="29" t="e">
         <f>F20/F21</f>
         <v>#NAME?</v>
       </c>
-      <c r="G22" s="22" t="e">
+      <c r="G22" s="29" t="e">
         <f>G20/G21</f>
         <v>#NAME?</v>
       </c>
@@ -1933,47 +1939,47 @@
       <c r="I22" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="22" t="e">
+      <c r="J22" s="29" t="e">
         <f>J20/J21</f>
         <v>#NAME?</v>
       </c>
-      <c r="K22" s="22" t="e">
+      <c r="K22" s="29" t="e">
         <f t="shared" ref="K22:N22" si="3">K20/K21</f>
         <v>#NAME?</v>
       </c>
-      <c r="L22" s="22" t="e">
+      <c r="L22" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
-      <c r="M22" s="22" t="e">
+      <c r="M22" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
-      <c r="N22" s="22" t="e">
+      <c r="N22" s="29" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="O22" s="13"/>
-      <c r="P22" s="23" t="s">
+      <c r="P22" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="Q22" s="25" t="e">
+      <c r="Q22" s="31" t="e">
         <f>Q20/Q21</f>
         <v>#NAME?</v>
       </c>
-      <c r="R22" s="25" t="e">
+      <c r="R22" s="31" t="e">
         <f t="shared" ref="R22:U22" si="4">R20/R21</f>
         <v>#NAME?</v>
       </c>
-      <c r="S22" s="25" t="e">
+      <c r="S22" s="31" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
-      <c r="T22" s="25" t="e">
+      <c r="T22" s="31" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
-      <c r="U22" s="25" t="e">
+      <c r="U22" s="31" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
@@ -1982,23 +1988,23 @@
       <c r="B23" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="22" t="e">
+      <c r="C23" s="29" t="e">
         <f>(1/C16)*C22</f>
         <v>#NAME?</v>
       </c>
-      <c r="D23" s="22" t="e">
+      <c r="D23" s="29" t="e">
         <f>(1/C16)*D22</f>
         <v>#NAME?</v>
       </c>
-      <c r="E23" s="22" t="e">
+      <c r="E23" s="29" t="e">
         <f>(1/C16)*E22</f>
         <v>#NAME?</v>
       </c>
-      <c r="F23" s="22" t="e">
+      <c r="F23" s="29" t="e">
         <f>(1/C16)*F22</f>
         <v>#NAME?</v>
       </c>
-      <c r="G23" s="22" t="e">
+      <c r="G23" s="29" t="e">
         <f>(1/C16)*G22</f>
         <v>#NAME?</v>
       </c>
@@ -2006,47 +2012,47 @@
       <c r="I23" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="J23" s="22" t="e">
+      <c r="J23" s="29" t="e">
         <f>(1/J16)*J22</f>
         <v>#NAME?</v>
       </c>
-      <c r="K23" s="22" t="e">
+      <c r="K23" s="29" t="e">
         <f>(1/J16)*K22</f>
         <v>#NAME?</v>
       </c>
-      <c r="L23" s="22" t="e">
+      <c r="L23" s="29" t="e">
         <f>(1/J16)*L22</f>
         <v>#NAME?</v>
       </c>
-      <c r="M23" s="22" t="e">
+      <c r="M23" s="29" t="e">
         <f>(1/J16)*M22</f>
         <v>#NAME?</v>
       </c>
-      <c r="N23" s="22" t="e">
+      <c r="N23" s="29" t="e">
         <f>(1/J16)*N22</f>
         <v>#NAME?</v>
       </c>
       <c r="O23" s="13"/>
-      <c r="P23" s="23" t="s">
+      <c r="P23" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="Q23" s="25" t="e">
+      <c r="Q23" s="31" t="e">
         <f>(1/Q16)*Q22</f>
         <v>#NAME?</v>
       </c>
-      <c r="R23" s="25" t="e">
+      <c r="R23" s="31" t="e">
         <f>(1/Q16)*R22</f>
         <v>#NAME?</v>
       </c>
-      <c r="S23" s="25" t="e">
+      <c r="S23" s="31" t="e">
         <f>(1/Q16)*S22</f>
         <v>#NAME?</v>
       </c>
-      <c r="T23" s="25" t="e">
+      <c r="T23" s="31" t="e">
         <f>(1/Q16)*T22</f>
         <v>#NAME?</v>
       </c>
-      <c r="U23" s="25" t="e">
+      <c r="U23" s="31" t="e">
         <f>(1/Q16/100)*U22</f>
         <v>#NAME?</v>
       </c>

</xml_diff>

<commit_message>
- Alguns ajustes nos KPIs - Resync com a possibilidade de apagar os actions
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -744,11 +744,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1443,7 +1443,10 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="13">
+        <f>10/(1+C5)</f>
+        <v>6.666666666666667</v>
+      </c>
       <c r="H11" s="13"/>
       <c r="I11" s="18" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
- Template. Esconder alguns campos quando nào tem dados
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -744,11 +744,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U23"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1118,7 +1118,7 @@
         <v>#NAME?</v>
       </c>
       <c r="M4" s="28" t="e">
-        <f>AVERAGE(Métricas!Primeira7dias7:Ultima7)</f>
+        <f>AVERAGE(Métricas!Primeiro_7dias7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
       <c r="N4" s="14"/>
@@ -1139,7 +1139,7 @@
         <v>#NAME?</v>
       </c>
       <c r="T4" s="30" t="e">
-        <f>AVERAGE(Métricas!Primeira3dias7:Ultima7)</f>
+        <f>AVERAGE(Métricas!Primeiro_3dias7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
       <c r="U4" s="13"/>
@@ -1443,16 +1443,13 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="13">
-        <f>10/(1+C5)</f>
-        <v>6.666666666666667</v>
-      </c>
+      <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="18" t="s">
         <v>43</v>
       </c>
       <c r="J11" s="29" t="e">
-        <f>IFERROR(SUM(Métricas!Primeira7dias5:Ultima5)/Venda_7dias,C11)</f>
+        <f>IFERROR(SUM(Métricas!Primeiro_7dias5:Ultima5)/Venda_7dias,C11)</f>
         <v>#NAME?</v>
       </c>
       <c r="K11" s="13"/>
@@ -1464,7 +1461,7 @@
         <v>43</v>
       </c>
       <c r="Q11" s="29" t="e">
-        <f>IFERROR(SUM(Métricas!Primeira3dias5:Ultima5)/Venda_3dias,C11)</f>
+        <f>IFERROR(SUM(Métricas!Primeiro_3dias5:Ultima5)/Venda_3dias,C11)</f>
         <v>#NAME?</v>
       </c>
       <c r="R11" s="13"/>
@@ -1637,7 +1634,7 @@
         <v>53</v>
       </c>
       <c r="J16" s="26" t="e">
-        <f>AVERAGE(Métricas!Primeira7dias6:Ultima6)/100</f>
+        <f>AVERAGE(Métricas!Primeiro_7dias6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
       <c r="K16" s="13"/>
@@ -1649,7 +1646,7 @@
         <v>53</v>
       </c>
       <c r="Q16" s="26" t="e">
-        <f>AVERAGE(Métricas!Primeira3dias6:Ultima6)/100</f>
+        <f>AVERAGE(Métricas!Primeiro_3dias6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
       <c r="R16" s="13"/>

</xml_diff>

<commit_message>
- Arrumando KPIs do Template - Colocando comissão e transação nos dados a serem associados - Validação para evitar duplicidade no dados a serem associados
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -973,7 +973,7 @@
   <dimension ref="B1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1089,7 +1089,7 @@
         <v>#NAME?</v>
       </c>
       <c r="D4" s="34" t="e">
-        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
       <c r="E4" s="28" t="e">
@@ -1152,7 +1152,7 @@
         <v>0.5</v>
       </c>
       <c r="D5" s="34" t="e">
-        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
       <c r="E5" s="28" t="e">
@@ -1213,7 +1213,7 @@
         <v>0.8</v>
       </c>
       <c r="D6" s="34" t="e">
-        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
       <c r="E6" s="28" t="e">
@@ -1274,7 +1274,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="34" t="e">
-        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
       <c r="E7" s="28" t="e">
@@ -1335,7 +1335,7 @@
         <v>1.2</v>
       </c>
       <c r="D8" s="34" t="e">
-        <f>IF(Vendas = 0, ViewContents, ViewContents/Vendas)</f>
+        <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
       <c r="E8" s="28" t="e">
@@ -1473,9 +1473,9 @@
       <c r="B12" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="26" t="e">
-        <f>Cartoes/Vendas</f>
-        <v>#NAME?</v>
+      <c r="C12" s="26">
+        <f>IFERROR(Cartoes/Vendas,0)</f>
+        <v>0</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -1510,9 +1510,9 @@
       <c r="B13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="26" t="e">
-        <f>BoletosPagos/Vendas</f>
-        <v>#NAME?</v>
+      <c r="C13" s="26">
+        <f>IFERROR(BoletosPagos/Vendas,0)</f>
+        <v>0</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
@@ -1547,9 +1547,9 @@
       <c r="B14" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="26" t="e">
-        <f>BoletosPagos/BoletosTotais</f>
-        <v>#NAME?</v>
+      <c r="C14" s="26">
+        <f>IFERROR(BoletosPagos/BoletosTotais,0)</f>
+        <v>0</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
@@ -1559,9 +1559,9 @@
       <c r="I14" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="J14" s="26" t="e">
+      <c r="J14" s="26">
         <f>IFERROR(Boletos_Pago_7dias/BoletosTotal_7dias,C14)</f>
-        <v>#NAME?</v>
+        <v>0</v>
       </c>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
@@ -1571,9 +1571,9 @@
       <c r="P14" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="Q14" s="26" t="e">
+      <c r="Q14" s="26">
         <f>IFERROR(Boletos_Pago_3dias/BoletosTotal_3dias,C14)</f>
-        <v>#NAME?</v>
+        <v>0</v>
       </c>
       <c r="R14" s="13"/>
       <c r="S14" s="13"/>
@@ -1585,7 +1585,7 @@
         <v>61</v>
       </c>
       <c r="C15" s="27" t="e">
-        <f>((1/D4)*C12)+((1/D4)*C13*C14)</f>
+        <f>IF(((1/D4)*C12)+((1/D4)*C13*C14)= 0, 0.005, ((1/D4)*C12)+((1/D4)*C13*C14))</f>
         <v>#NAME?</v>
       </c>
       <c r="D15" s="13"/>
@@ -1709,7 +1709,7 @@
         <v>41</v>
       </c>
       <c r="C19" s="26" t="e">
-        <f>(30/C11)-1</f>
+        <f>(comissao/C11)-1</f>
         <v>#NAME?</v>
       </c>
       <c r="D19" s="22">

</xml_diff>

<commit_message>
- Arrumando CPV na planilha - Formatação um pouco melhor do template
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
   <si>
     <t>Dia:</t>
   </si>
@@ -132,9 +132,6 @@
     <t>#boletos_pagos</t>
   </si>
   <si>
-    <t>#cartoes</t>
-  </si>
-  <si>
     <t>#faturamento_boleto</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>Meta 3</t>
   </si>
   <si>
-    <t>LPV</t>
-  </si>
-  <si>
     <t>% Cartões</t>
   </si>
   <si>
@@ -201,19 +195,37 @@
     <t>Este anúncio</t>
   </si>
   <si>
-    <t>Vitalício</t>
-  </si>
-  <si>
-    <t>Última semana</t>
-  </si>
-  <si>
-    <t>Últimos três dias</t>
-  </si>
-  <si>
     <t>Meta 4</t>
   </si>
   <si>
     <t>Taxa Conversao</t>
+  </si>
+  <si>
+    <t>Anúncio Atual</t>
+  </si>
+  <si>
+    <t>ROI Projetado</t>
+  </si>
+  <si>
+    <t>KPI Baseado na Última semana</t>
+  </si>
+  <si>
+    <t>KPI Baseado no Dados Vitalícios</t>
+  </si>
+  <si>
+    <t>KPI nos Últimos três dias</t>
+  </si>
+  <si>
+    <t>ROI Metas</t>
+  </si>
+  <si>
+    <t>CPC Atual</t>
+  </si>
+  <si>
+    <t>CPV Projetado</t>
+  </si>
+  <si>
+    <t>CPV Meta</t>
   </si>
 </sst>
 </file>
@@ -391,7 +403,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -435,6 +447,15 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -748,7 +769,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -763,7 +784,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
@@ -861,7 +882,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
@@ -885,7 +906,7 @@
         <v>31</v>
       </c>
       <c r="B17" s="10" t="str">
-        <f>IFERROR(ROUND($B5/($B12+$B15),2),"")</f>
+        <f>IFERROR(ROUND($B5/Vendas,2),"")</f>
         <v/>
       </c>
     </row>
@@ -894,7 +915,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
@@ -902,7 +923,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
@@ -941,7 +962,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
@@ -949,7 +970,7 @@
         <v>20</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
@@ -957,7 +978,7 @@
         <v>21</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -970,10 +991,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U23"/>
+  <dimension ref="B1:U24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -986,7 +1007,7 @@
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B1" s="13" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -995,7 +1016,7 @@
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
       <c r="I1" s="13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J1" s="13"/>
       <c r="K1" s="13"/>
@@ -1004,7 +1025,7 @@
       <c r="N1" s="13"/>
       <c r="O1" s="13"/>
       <c r="P1" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
@@ -1037,52 +1058,52 @@
     <row r="3" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B3" s="14"/>
       <c r="C3" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>42</v>
-      </c>
       <c r="E3" s="15" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="13"/>
       <c r="I3" s="14"/>
       <c r="J3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>42</v>
-      </c>
       <c r="L3" s="15" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="N3" s="16"/>
       <c r="O3" s="13"/>
       <c r="P3" s="14"/>
       <c r="Q3" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="17" t="s">
-        <v>44</v>
+      <c r="S3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>63</v>
       </c>
       <c r="U3" s="13"/>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B4" s="18" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C4" s="24" t="e">
         <f>(comissao/E4)-1</f>
@@ -1103,7 +1124,7 @@
       <c r="G4" s="14"/>
       <c r="H4" s="13"/>
       <c r="I4" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J4" s="24" t="e">
         <f>(comissao/L4)-1</f>
@@ -1124,7 +1145,7 @@
       <c r="N4" s="14"/>
       <c r="O4" s="13"/>
       <c r="P4" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="25" t="e">
         <f>(comissao/S4)-1</f>
@@ -1145,72 +1166,57 @@
       <c r="U4" s="13"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B5" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="34" t="e">
-        <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E5" s="28" t="e">
-        <f>comissao/(1+C5)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F5" s="28" t="e">
-        <f>E5/D5</f>
-        <v>#NAME?</v>
+      <c r="B5" s="18"/>
+      <c r="C5" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="39" t="s">
+        <v>43</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="13"/>
-      <c r="I5" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="K5" s="34" t="e">
-        <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L5" s="28" t="e">
-        <f>comissao/(1+J5)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M5" s="28" t="e">
-        <f>L5/K5</f>
-        <v>#NAME?</v>
+      <c r="I5" s="18"/>
+      <c r="J5" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="M5" s="39" t="s">
+        <v>43</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="13"/>
-      <c r="P5" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q5" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="R5" s="35" t="e">
-        <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="S5" s="30" t="e">
-        <f>comissao/(Q5+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="T5" s="30" t="e">
-        <f>S5/R5</f>
-        <v>#NAME?</v>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="T5" s="39" t="s">
+        <v>43</v>
       </c>
       <c r="U5" s="13"/>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B6" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C6" s="19">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="34" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
@@ -1221,16 +1227,16 @@
         <v>#NAME?</v>
       </c>
       <c r="F6" s="28" t="e">
-        <f t="shared" ref="F6:F8" si="0">E6/D6</f>
+        <f>E6/D6</f>
         <v>#NAME?</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="13"/>
       <c r="I6" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="J6" s="19">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="K6" s="34" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
@@ -1241,16 +1247,16 @@
         <v>#NAME?</v>
       </c>
       <c r="M6" s="28" t="e">
-        <f t="shared" ref="M6:M8" si="1">L6/K6</f>
+        <f>L6/K6</f>
         <v>#NAME?</v>
       </c>
       <c r="N6" s="14"/>
       <c r="O6" s="13"/>
       <c r="P6" s="18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="Q6" s="19">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="R6" s="35" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
@@ -1261,17 +1267,17 @@
         <v>#NAME?</v>
       </c>
       <c r="T6" s="30" t="e">
-        <f t="shared" ref="T6:T8" si="2">S6/R6</f>
+        <f>S6/R6</f>
         <v>#NAME?</v>
       </c>
       <c r="U6" s="13"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B7" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="19">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D7" s="34" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
@@ -1282,16 +1288,16 @@
         <v>#NAME?</v>
       </c>
       <c r="F7" s="28" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F7:F9" si="0">E7/D7</f>
         <v>#NAME?</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="13"/>
       <c r="I7" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J7" s="19">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="K7" s="34" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
@@ -1302,16 +1308,16 @@
         <v>#NAME?</v>
       </c>
       <c r="M7" s="28" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="M7:M9" si="1">L7/K7</f>
         <v>#NAME?</v>
       </c>
       <c r="N7" s="14"/>
       <c r="O7" s="13"/>
       <c r="P7" s="18" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q7" s="19">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="R7" s="35" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
@@ -1322,17 +1328,17 @@
         <v>#NAME?</v>
       </c>
       <c r="T7" s="30" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="T7:T9" si="2">S7/R7</f>
         <v>#NAME?</v>
       </c>
       <c r="U7" s="13"/>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B8" s="18" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C8" s="19">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="34" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
@@ -1349,10 +1355,10 @@
       <c r="G8" s="14"/>
       <c r="H8" s="13"/>
       <c r="I8" s="18" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="J8" s="19">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="34" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
@@ -1369,10 +1375,10 @@
       <c r="N8" s="14"/>
       <c r="O8" s="13"/>
       <c r="P8" s="18" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="Q8" s="19">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="R8" s="35" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
@@ -1389,25 +1395,64 @@
       <c r="U8" s="13"/>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="D9" s="34" t="e">
+        <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E9" s="28" t="e">
+        <f>comissao/(1+C9)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F9" s="28" t="e">
+        <f t="shared" si="0"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="G9" s="14"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
+      <c r="I9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="K9" s="34" t="e">
+        <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L9" s="28" t="e">
+        <f>comissao/(1+J9)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M9" s="28" t="e">
+        <f t="shared" si="1"/>
+        <v>#NAME?</v>
+      </c>
+      <c r="N9" s="14"/>
       <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
+      <c r="P9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="19">
+        <v>1.2</v>
+      </c>
+      <c r="R9" s="35" t="e">
+        <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S9" s="30" t="e">
+        <f>comissao/(Q9+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T9" s="30" t="e">
+        <f t="shared" si="2"/>
+        <v>#NAME?</v>
+      </c>
       <c r="U9" s="13"/>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.2">
@@ -1433,37 +1478,22 @@
       <c r="U10" s="13"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B11" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="29" t="e">
-        <f>IF(Vendas = 0, E4, Métricas!Geral5/Vendas)</f>
-        <v>#NAME?</v>
-      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
-      <c r="I11" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" s="29" t="e">
-        <f>IFERROR(SUM(Métricas!Primeiro_7dias5:Ultima5)/Venda_7dias,C11)</f>
-        <v>#NAME?</v>
-      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
-      <c r="P11" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q11" s="29" t="e">
-        <f>IFERROR(SUM(Métricas!Primeiro_3dias5:Ultima5)/Venda_3dias,C11)</f>
-        <v>#NAME?</v>
-      </c>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
       <c r="S11" s="13"/>
       <c r="T11" s="13"/>
@@ -1471,11 +1501,11 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B12" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="26">
-        <f>IFERROR(Cartoes/Vendas,0)</f>
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="C12" s="29" t="e">
+        <f>IF(Vendas = 0, E4, Métricas!Geral5/Vendas)</f>
+        <v>#NAME?</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -1483,23 +1513,23 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="J12" s="26">
-        <f>IFERROR(Cartao_7dias/Venda_7dias,0)</f>
-        <v>0</v>
+        <v>42</v>
+      </c>
+      <c r="J12" s="29" t="e">
+        <f>IFERROR(SUM(Métricas!Primeiro_7dias5:Ultima5)/Venda_7dias,C12)</f>
+        <v>#NAME?</v>
       </c>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
       <c r="O12" s="13"/>
-      <c r="P12" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q12" s="26">
-        <f>IFERROR(Cartao_3dias/Venda_3dias,0)</f>
-        <v>0</v>
+      <c r="P12" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" s="29" t="e">
+        <f>IFERROR(SUM(Métricas!Primeiro_3dias5:Ultima5)/Venda_3dias,C12)</f>
+        <v>#NAME?</v>
       </c>
       <c r="R12" s="13"/>
       <c r="S12" s="13"/>
@@ -1508,10 +1538,10 @@
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B13" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13" s="26">
-        <f>IFERROR(BoletosPagos/Vendas,0)</f>
+        <f>IFERROR(Cartoes/Vendas,0)</f>
         <v>0</v>
       </c>
       <c r="D13" s="13"/>
@@ -1520,10 +1550,10 @@
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
       <c r="I13" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J13" s="26">
-        <f>IFERROR(BoletosPago_7dias/Venda_7dias,0)</f>
+        <f>IFERROR(Cartao_7dias/Venda_7dias,0)</f>
         <v>0</v>
       </c>
       <c r="K13" s="13"/>
@@ -1532,10 +1562,10 @@
       <c r="N13" s="13"/>
       <c r="O13" s="13"/>
       <c r="P13" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="Q13" s="26">
-        <f>IFERROR(BoletosPago_3dias/Venda_3dias,0)</f>
+        <f>IFERROR(Cartao_3dias/Venda_3dias,0)</f>
         <v>0</v>
       </c>
       <c r="R13" s="13"/>
@@ -1545,10 +1575,10 @@
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B14" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C14" s="26">
-        <f>IFERROR(BoletosPagos/BoletosTotais,0)</f>
+        <f>IFERROR(BoletosPagos/Vendas,0)</f>
         <v>0</v>
       </c>
       <c r="D14" s="13"/>
@@ -1557,10 +1587,10 @@
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J14" s="26">
-        <f>IFERROR(Boletos_Pago_7dias/BoletosTotal_7dias,C14)</f>
+        <f>IFERROR(BoletosPago_7dias/Venda_7dias,0)</f>
         <v>0</v>
       </c>
       <c r="K14" s="13"/>
@@ -1569,10 +1599,10 @@
       <c r="N14" s="13"/>
       <c r="O14" s="13"/>
       <c r="P14" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q14" s="26">
-        <f>IFERROR(Boletos_Pago_3dias/BoletosTotal_3dias,C14)</f>
+        <f>IFERROR(BoletosPago_3dias/Venda_3dias,0)</f>
         <v>0</v>
       </c>
       <c r="R14" s="13"/>
@@ -1582,11 +1612,11 @@
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B15" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="27" t="e">
-        <f>IF(((1/D4)*C12)+((1/D4)*C13*C14)= 0, 0.005, ((1/D4)*C12)+((1/D4)*C13*C14))</f>
-        <v>#NAME?</v>
+        <v>50</v>
+      </c>
+      <c r="C15" s="26">
+        <f>IFERROR(BoletosPagos/BoletosTotais,0)</f>
+        <v>0</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
@@ -1594,23 +1624,23 @@
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="27" t="e">
-        <f>IF(IFERROR(((1/K4)*J12)+((1/K4)*J13*J14),C15)=0,C15,IFERROR(((1/K4)*J12)+((1/K4)*J13*J14),C15))</f>
-        <v>#NAME?</v>
+        <v>50</v>
+      </c>
+      <c r="J15" s="26">
+        <f>IFERROR(Boletos_Pago_7dias/BoletosTotal_7dias,C15)</f>
+        <v>0</v>
       </c>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
-      <c r="P15" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q15" s="27" t="e">
-        <f>IF(IFERROR(((1/R4)*Q12)+((1/R4)*Q13*Q14),C15)=0,C15,IFERROR(((1/R4)*Q12)+((1/R4)*Q13*Q14),C15))</f>
-        <v>#NAME?</v>
+      <c r="P15" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="26">
+        <f>IFERROR(Boletos_Pago_3dias/BoletosTotal_3dias,C15)</f>
+        <v>0</v>
       </c>
       <c r="R15" s="13"/>
       <c r="S15" s="13"/>
@@ -1619,10 +1649,10 @@
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B16" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="26" t="e">
-        <f>AVERAGE(Métricas!Primeira6:Ultima6)/100</f>
+        <v>56</v>
+      </c>
+      <c r="C16" s="27" t="e">
+        <f>IF(((1/D4)*C13)+((1/D4)*C14*C15)= 0, 0.005, ((1/D4)*C13)+((1/D4)*C14*C15))</f>
         <v>#NAME?</v>
       </c>
       <c r="D16" s="13"/>
@@ -1631,10 +1661,10 @@
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
       <c r="I16" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="J16" s="26" t="e">
-        <f>AVERAGE(Métricas!Primeiro_7dias6:Ultima6)/100</f>
+        <v>56</v>
+      </c>
+      <c r="J16" s="27" t="e">
+        <f>IF(IFERROR(((1/K4)*J13)+((1/K4)*J14*J15),C16)=0,C16,IFERROR(((1/K4)*J13)+((1/K4)*J14*J15),C16))</f>
         <v>#NAME?</v>
       </c>
       <c r="K16" s="13"/>
@@ -1642,11 +1672,11 @@
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
       <c r="O16" s="13"/>
-      <c r="P16" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q16" s="26" t="e">
-        <f>AVERAGE(Métricas!Primeiro_3dias6:Ultima6)/100</f>
+      <c r="P16" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q16" s="27" t="e">
+        <f>IF(IFERROR(((1/R4)*Q13)+((1/R4)*Q14*Q15),C16)=0,C16,IFERROR(((1/R4)*Q13)+((1/R4)*Q14*Q15),C16))</f>
         <v>#NAME?</v>
       </c>
       <c r="R16" s="13"/>
@@ -1655,22 +1685,37 @@
       <c r="U16" s="13"/>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
+      <c r="B17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="26" t="e">
+        <f>AVERAGE(Métricas!Primeira6:Ultima6)/100</f>
+        <v>#NAME?</v>
+      </c>
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+      <c r="I17" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="26" t="e">
+        <f>AVERAGE(Métricas!Primeiro_7dias6:Ultima6)/100</f>
+        <v>#NAME?</v>
+      </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
       <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
+      <c r="P17" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q17" s="26" t="e">
+        <f>AVERAGE(Métricas!Primeiro_3dias6:Ultima6)/100</f>
+        <v>#NAME?</v>
+      </c>
       <c r="R17" s="13"/>
       <c r="S17" s="13"/>
       <c r="T17" s="13"/>
@@ -1678,382 +1723,404 @@
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B18" s="13"/>
-      <c r="C18" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="C18" s="13"/>
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
-      <c r="J18" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
       <c r="O18" s="13"/>
       <c r="P18" s="13"/>
-      <c r="Q18" s="20" t="s">
-        <v>56</v>
-      </c>
+      <c r="Q18" s="13"/>
       <c r="R18" s="13"/>
       <c r="S18" s="13"/>
       <c r="T18" s="13"/>
       <c r="U18" s="13"/>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.2">
-      <c r="B19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="26" t="e">
-        <f>(comissao/C11)-1</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D19" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="E19" s="22">
-        <v>0.8</v>
-      </c>
-      <c r="F19" s="22">
-        <v>1</v>
-      </c>
-      <c r="G19" s="22">
-        <v>1.2</v>
-      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="26">
-        <f>IFERROR((comissao/J11)-1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="22">
-        <v>0.5</v>
-      </c>
-      <c r="L19" s="22">
-        <v>0.8</v>
-      </c>
-      <c r="M19" s="22">
-        <v>1</v>
-      </c>
-      <c r="N19" s="22">
-        <v>1.2</v>
-      </c>
+      <c r="I19" s="13"/>
+      <c r="J19" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
       <c r="O19" s="13"/>
-      <c r="P19" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q19" s="36">
-        <f>IFERROR((comissao/Q11)-1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="R19" s="23">
-        <v>0.5</v>
-      </c>
-      <c r="S19" s="23">
-        <v>0.8</v>
-      </c>
-      <c r="T19" s="23">
-        <v>1</v>
-      </c>
-      <c r="U19" s="23">
-        <v>1.2</v>
-      </c>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B20" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="29" t="e">
-        <f>C11</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D20" s="29" t="e">
-        <f>comissao/(D19+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E20" s="29" t="e">
-        <f>comissao/(E19+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F20" s="29" t="e">
-        <f>comissao/(F19+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G20" s="29" t="e">
-        <f>comissao/(G19+1)</f>
-        <v>#NAME?</v>
+        <v>40</v>
+      </c>
+      <c r="C20" s="26" t="e">
+        <f>(comissao/C12)-1</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D20" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="F20" s="22">
+        <v>1</v>
+      </c>
+      <c r="G20" s="22">
+        <v>1.2</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="J20" s="29" t="e">
-        <f>J11</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K20" s="29" t="e">
-        <f>comissao/(K19+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L20" s="29" t="e">
-        <f>comissao/(L19+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M20" s="29" t="e">
-        <f>comissao/(M19+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N20" s="29" t="e">
-        <f>comissao/(N19+1)</f>
-        <v>#NAME?</v>
+        <v>40</v>
+      </c>
+      <c r="J20" s="26">
+        <f>IFERROR((comissao/J12)-1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="L20" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="M20" s="22">
+        <v>1</v>
+      </c>
+      <c r="N20" s="22">
+        <v>1.2</v>
       </c>
       <c r="O20" s="13"/>
-      <c r="P20" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q20" s="31" t="e">
-        <f>Q11</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="R20" s="31" t="e">
-        <f>comissao/(R19+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="S20" s="31" t="e">
-        <f>comissao/(S19+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="T20" s="31" t="e">
-        <f>comissao/(T19+1)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="U20" s="31" t="e">
-        <f>comissao/(U19+1)</f>
-        <v>#NAME?</v>
+      <c r="P20" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q20" s="36">
+        <f>IFERROR((comissao/Q12)-1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="R20" s="23">
+        <v>0.5</v>
+      </c>
+      <c r="S20" s="23">
+        <v>0.8</v>
+      </c>
+      <c r="T20" s="23">
+        <v>1</v>
+      </c>
+      <c r="U20" s="23">
+        <v>1.2</v>
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B21" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="33" t="e">
-        <f>1/C15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D21" s="33" t="e">
-        <f>1/C15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E21" s="33" t="e">
-        <f>1/C15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F21" s="33" t="e">
-        <f>1/C15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G21" s="33" t="e">
-        <f>1/C15</f>
+        <v>42</v>
+      </c>
+      <c r="C21" s="29" t="e">
+        <f>C12</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D21" s="29" t="e">
+        <f>comissao/(D20+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E21" s="29" t="e">
+        <f>comissao/(E20+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F21" s="29" t="e">
+        <f>comissao/(F20+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G21" s="29" t="e">
+        <f>comissao/(G20+1)</f>
         <v>#NAME?</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="J21" s="33" t="e">
-        <f>1/J15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K21" s="33" t="e">
-        <f>1/J15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L21" s="33" t="e">
-        <f>1/J15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M21" s="33" t="e">
-        <f>1/J15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N21" s="33" t="e">
-        <f>1/J15</f>
+        <v>42</v>
+      </c>
+      <c r="J21" s="29" t="e">
+        <f>J12</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K21" s="29" t="e">
+        <f>comissao/(K20+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L21" s="29" t="e">
+        <f>comissao/(L20+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M21" s="29" t="e">
+        <f>comissao/(M20+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N21" s="29" t="e">
+        <f>comissao/(N20+1)</f>
         <v>#NAME?</v>
       </c>
       <c r="O21" s="13"/>
       <c r="P21" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q21" s="32" t="e">
-        <f>1/Q15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="R21" s="32" t="e">
-        <f>1/Q15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="S21" s="32" t="e">
-        <f>1/Q15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="T21" s="32" t="e">
-        <f>1/Q15</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="U21" s="32" t="e">
-        <f>1/Q15</f>
+        <v>42</v>
+      </c>
+      <c r="Q21" s="31" t="e">
+        <f>Q12</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R21" s="31" t="e">
+        <f>comissao/(R20+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S21" s="31" t="e">
+        <f>comissao/(S20+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T21" s="31" t="e">
+        <f>comissao/(T20+1)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U21" s="31" t="e">
+        <f>comissao/(U20+1)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B22" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="29" t="e">
-        <f>C20/C21</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D22" s="29" t="e">
-        <f>D20/D21</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="E22" s="29" t="e">
-        <f>E20/E21</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="F22" s="29" t="e">
-        <f>F20/F21</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="G22" s="29" t="e">
-        <f>G20/G21</f>
+        <v>41</v>
+      </c>
+      <c r="C22" s="33" t="e">
+        <f>1/C16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D22" s="33" t="e">
+        <f>1/C16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E22" s="33" t="e">
+        <f>1/C16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F22" s="33" t="e">
+        <f>1/C16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G22" s="33" t="e">
+        <f>1/C16</f>
         <v>#NAME?</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="J22" s="29" t="e">
-        <f>J20/J21</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K22" s="29" t="e">
-        <f t="shared" ref="K22:N22" si="3">K20/K21</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L22" s="29" t="e">
-        <f t="shared" si="3"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="M22" s="29" t="e">
-        <f t="shared" si="3"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="N22" s="29" t="e">
-        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="J22" s="33" t="e">
+        <f>1/J16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K22" s="33" t="e">
+        <f>1/J16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L22" s="33" t="e">
+        <f>1/J16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M22" s="33" t="e">
+        <f>1/J16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N22" s="33" t="e">
+        <f>1/J16</f>
         <v>#NAME?</v>
       </c>
       <c r="O22" s="13"/>
-      <c r="P22" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q22" s="31" t="e">
-        <f>Q20/Q21</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="R22" s="31" t="e">
-        <f t="shared" ref="R22:U22" si="4">R20/R21</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="S22" s="31" t="e">
-        <f t="shared" si="4"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="T22" s="31" t="e">
-        <f t="shared" si="4"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="U22" s="31" t="e">
-        <f t="shared" si="4"/>
+      <c r="P22" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q22" s="32" t="e">
+        <f>1/Q16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R22" s="32" t="e">
+        <f>1/Q16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S22" s="32" t="e">
+        <f>1/Q16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T22" s="32" t="e">
+        <f>1/Q16</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U22" s="32" t="e">
+        <f>1/Q16</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B23" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C23" s="29" t="e">
-        <f>(1/C16)*C22</f>
+        <f>C21/C22</f>
         <v>#NAME?</v>
       </c>
       <c r="D23" s="29" t="e">
-        <f>(1/C16)*D22</f>
+        <f>D21/D22</f>
         <v>#NAME?</v>
       </c>
       <c r="E23" s="29" t="e">
-        <f>(1/C16)*E22</f>
+        <f>E21/E22</f>
         <v>#NAME?</v>
       </c>
       <c r="F23" s="29" t="e">
-        <f>(1/C16)*F22</f>
+        <f>F21/F22</f>
         <v>#NAME?</v>
       </c>
       <c r="G23" s="29" t="e">
-        <f>(1/C16)*G22</f>
+        <f>G21/G22</f>
         <v>#NAME?</v>
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J23" s="29" t="e">
-        <f>(1/J16)*J22</f>
+        <f>J21/J22</f>
         <v>#NAME?</v>
       </c>
       <c r="K23" s="29" t="e">
-        <f>(1/J16)*K22</f>
+        <f t="shared" ref="K23:N23" si="3">K21/K22</f>
         <v>#NAME?</v>
       </c>
       <c r="L23" s="29" t="e">
-        <f>(1/J16)*L22</f>
+        <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="M23" s="29" t="e">
-        <f>(1/J16)*M22</f>
+        <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="N23" s="29" t="e">
-        <f>(1/J16)*N22</f>
+        <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="O23" s="13"/>
       <c r="P23" s="21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q23" s="31" t="e">
-        <f>(1/Q16)*Q22</f>
+        <f>Q21/Q22</f>
         <v>#NAME?</v>
       </c>
       <c r="R23" s="31" t="e">
-        <f>(1/Q16)*R22</f>
+        <f t="shared" ref="R23:U23" si="4">R21/R22</f>
         <v>#NAME?</v>
       </c>
       <c r="S23" s="31" t="e">
-        <f>(1/Q16)*S22</f>
+        <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="T23" s="31" t="e">
-        <f>(1/Q16)*T22</f>
+        <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
       <c r="U23" s="31" t="e">
-        <f>(1/Q16/100)*U22</f>
+        <f t="shared" si="4"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="29" t="e">
+        <f>(1/C17)*C23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="D24" s="29" t="e">
+        <f>(1/C17)*D23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="E24" s="29" t="e">
+        <f>(1/C17)*E23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="F24" s="29" t="e">
+        <f>(1/C17)*F23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="G24" s="29" t="e">
+        <f>(1/C17)*G23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H24" s="13"/>
+      <c r="I24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="J24" s="29" t="e">
+        <f>(1/J17)*J23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="K24" s="29" t="e">
+        <f>(1/J17)*K23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="L24" s="29" t="e">
+        <f>(1/J17)*L23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="M24" s="29" t="e">
+        <f>(1/J17)*M23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="N24" s="29" t="e">
+        <f>(1/J17)*N23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O24" s="13"/>
+      <c r="P24" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q24" s="31" t="e">
+        <f>(1/Q17)*Q23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="R24" s="31" t="e">
+        <f>(1/Q17)*R23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="S24" s="31" t="e">
+        <f>(1/Q17)*S23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="T24" s="31" t="e">
+        <f>(1/Q17)*T23</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="U24" s="31" t="e">
+        <f>(1/Q17/100)*U23</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Cartoes no template deixou de funcionar
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
   <si>
     <t>Dia:</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>CPV Meta</t>
+  </si>
+  <si>
+    <t>#cartoes</t>
   </si>
 </sst>
 </file>
@@ -765,11 +768,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -882,7 +885,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
@@ -993,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
- Salvando informações das contas de account_info - Pegando informações de ads_vendas para mostrar informações de anúncios vendedores
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="81">
   <si>
     <t>Dia:</t>
   </si>
@@ -229,6 +229,48 @@
   </si>
   <si>
     <t>#cartoes</t>
+  </si>
+  <si>
+    <t>%Boletos</t>
+  </si>
+  <si>
+    <t>Taxa Conversão</t>
+  </si>
+  <si>
+    <t>Métricas que estão vendendo para esse produto</t>
+  </si>
+  <si>
+    <t>cpv_venda</t>
+  </si>
+  <si>
+    <t>boletos_venda</t>
+  </si>
+  <si>
+    <t>cartoes_venda</t>
+  </si>
+  <si>
+    <t>conv_boleto_venda</t>
+  </si>
+  <si>
+    <t>ctr_venda</t>
+  </si>
+  <si>
+    <t>cpc_venda</t>
+  </si>
+  <si>
+    <t>cpm_venda</t>
+  </si>
+  <si>
+    <t>roi_venda</t>
+  </si>
+  <si>
+    <t>clpv_venda</t>
+  </si>
+  <si>
+    <t>Investimento</t>
+  </si>
+  <si>
+    <t>spend_venda</t>
   </si>
 </sst>
 </file>
@@ -406,7 +448,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -459,6 +501,11 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -768,7 +815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -994,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:U24"/>
+  <dimension ref="B1:U38"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2127,6 +2174,100 @@
         <v>#NAME?</v>
       </c>
     </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B27" s="40" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B28" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B29" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B30" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B31" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="42" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B32" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="42" t="e">
+        <f>IF(((1/C34)*C29)+((1/C34)*C30*C31)= 0, 0.005, ((1/C34)*C29)+((1/C34)*C30*C31))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="43" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- Algumas métricas no Template para comparação de números a outras campanhas - Erro ao associar postback
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -813,23 +813,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="25.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.83203125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="2"/>
+    <col min="2" max="2" width="8.83203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -837,7 +837,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -845,7 +845,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -853,7 +853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -861,7 +861,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -869,7 +869,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -877,7 +877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -885,7 +885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
@@ -893,7 +893,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
@@ -901,15 +901,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
-      <c r="G10" s="2" t="str">
-        <f>IFERROR(AVERAGE(A1:A2),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
@@ -917,17 +913,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="6"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -935,7 +931,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>12</v>
       </c>
@@ -943,7 +939,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16" s="9" t="s">
         <v>13</v>
       </c>
@@ -1043,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
- Atualizaçào de tab - Download de planilha
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -1144,7 +1144,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1158,7 +1157,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1170,7 +1168,6 @@
     <xf numFmtId="2" fontId="2" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1215,9 +1212,6 @@
     <xf numFmtId="1" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="12" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="12" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1252,9 +1246,6 @@
     <xf numFmtId="2" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="13" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="13" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1285,9 +1276,6 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="14" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="14" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="2" fillId="14" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1339,6 +1327,18 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="14" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="14" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="2" fillId="14" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="13" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="12" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1346,7 +1346,25 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1652,7 +1670,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -1873,7 +1891,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+      <selection activeCell="C25" activeCellId="5" sqref="C5 J5 Q5 Q25 J25 C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1891,7 +1909,7 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="128" t="s">
         <v>78</v>
       </c>
       <c r="C2" s="14"/>
@@ -1900,7 +1918,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="71" t="s">
         <v>79</v>
       </c>
       <c r="J2" s="14"/>
@@ -1909,7 +1927,7 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
-      <c r="P2" s="73" t="s">
+      <c r="P2" s="70" t="s">
         <v>80</v>
       </c>
       <c r="Q2" s="14"/>
@@ -1920,1236 +1938,1236 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="135"/>
-      <c r="C3" s="136"/>
-      <c r="D3" s="136"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="136"/>
-      <c r="G3" s="137"/>
+      <c r="B3" s="129"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="131"/>
       <c r="H3" s="14"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="77"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+      <c r="L3" s="73"/>
+      <c r="M3" s="73"/>
+      <c r="N3" s="74"/>
       <c r="O3" s="14"/>
-      <c r="P3" s="163"/>
-      <c r="Q3" s="62"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="62"/>
-      <c r="T3" s="62"/>
-      <c r="U3" s="63"/>
+      <c r="P3" s="157"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="60"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="138"/>
-      <c r="C4" s="98" t="s">
+      <c r="B4" s="132"/>
+      <c r="C4" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="98" t="s">
+      <c r="D4" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="98" t="s">
+      <c r="E4" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="98" t="s">
+      <c r="F4" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="139"/>
+      <c r="G4" s="133"/>
       <c r="H4" s="14"/>
-      <c r="I4" s="78"/>
-      <c r="J4" s="99" t="s">
+      <c r="I4" s="75"/>
+      <c r="J4" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="99" t="s">
+      <c r="K4" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="99" t="s">
+      <c r="L4" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="99" t="s">
+      <c r="M4" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="N4" s="79"/>
+      <c r="N4" s="76"/>
       <c r="O4" s="14"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="113" t="s">
+      <c r="P4" s="61"/>
+      <c r="Q4" s="108" t="s">
         <v>58</v>
       </c>
-      <c r="R4" s="114" t="s">
+      <c r="R4" s="109" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="113" t="s">
+      <c r="S4" s="108" t="s">
         <v>61</v>
       </c>
-      <c r="T4" s="113" t="s">
+      <c r="T4" s="108" t="s">
         <v>60</v>
       </c>
-      <c r="U4" s="65"/>
+      <c r="U4" s="62"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="25" t="e">
+      <c r="C5" s="164" t="e">
         <f>(comissao/E5)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="D5" s="26" t="e">
+      <c r="D5" s="25" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E5" s="27" t="e">
+      <c r="E5" s="26" t="e">
         <f>F5*D5</f>
         <v>#NAME?</v>
       </c>
-      <c r="F5" s="27" t="e">
+      <c r="F5" s="26" t="e">
         <f>AVERAGE(Métricas!Primeira7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
-      <c r="G5" s="141"/>
+      <c r="G5" s="135"/>
       <c r="H5" s="14"/>
-      <c r="I5" s="80" t="s">
+      <c r="I5" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="37" t="e">
+      <c r="J5" s="165" t="e">
         <f>(comissao/L5)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="K5" s="38" t="e">
+      <c r="K5" s="36" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L5" s="39" t="e">
+      <c r="L5" s="37" t="e">
         <f>M5*K5</f>
         <v>#NAME?</v>
       </c>
-      <c r="M5" s="39" t="e">
+      <c r="M5" s="37" t="e">
         <f>AVERAGE(Métricas!Primeiro_7dias7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N5" s="81"/>
+      <c r="N5" s="78"/>
       <c r="O5" s="14"/>
-      <c r="P5" s="66" t="s">
+      <c r="P5" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="Q5" s="49" t="e">
+      <c r="Q5" s="166" t="e">
         <f>(comissao/S5)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="R5" s="50" t="e">
+      <c r="R5" s="47" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S5" s="51" t="e">
+      <c r="S5" s="48" t="e">
         <f>T5*R5</f>
         <v>#NAME?</v>
       </c>
-      <c r="T5" s="51" t="e">
+      <c r="T5" s="48" t="e">
         <f>AVERAGE(Métricas!Primeiro_3dias7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
-      <c r="U5" s="65"/>
-    </row>
-    <row r="6" spans="1:21" s="59" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U5" s="62"/>
+    </row>
+    <row r="6" spans="1:21" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="23"/>
-      <c r="B6" s="142"/>
+      <c r="B6" s="136"/>
       <c r="C6" s="20"/>
       <c r="D6" s="21"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
-      <c r="G6" s="143"/>
+      <c r="G6" s="137"/>
       <c r="H6" s="23"/>
-      <c r="I6" s="82"/>
+      <c r="I6" s="79"/>
       <c r="J6" s="20"/>
       <c r="K6" s="21"/>
       <c r="L6" s="22"/>
       <c r="M6" s="22"/>
-      <c r="N6" s="83"/>
+      <c r="N6" s="80"/>
       <c r="O6" s="23"/>
-      <c r="P6" s="67"/>
+      <c r="P6" s="64"/>
       <c r="Q6" s="20"/>
       <c r="R6" s="21"/>
       <c r="S6" s="22"/>
       <c r="T6" s="22"/>
-      <c r="U6" s="68"/>
+      <c r="U6" s="65"/>
     </row>
     <row r="7" spans="1:21" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="57" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="142"/>
+      <c r="B7" s="136"/>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
-      <c r="G7" s="143"/>
+      <c r="G7" s="137"/>
       <c r="H7" s="23"/>
-      <c r="I7" s="82"/>
+      <c r="I7" s="79"/>
       <c r="J7" s="20"/>
       <c r="K7" s="21"/>
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
-      <c r="N7" s="83"/>
+      <c r="N7" s="80"/>
       <c r="O7" s="23"/>
-      <c r="P7" s="67"/>
+      <c r="P7" s="64"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="21"/>
       <c r="S7" s="22"/>
       <c r="T7" s="22"/>
-      <c r="U7" s="68"/>
-    </row>
-    <row r="8" spans="1:21" s="59" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="60"/>
-      <c r="B8" s="142"/>
+      <c r="U7" s="65"/>
+    </row>
+    <row r="8" spans="1:21" s="56" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="57"/>
+      <c r="B8" s="136"/>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
-      <c r="G8" s="143"/>
+      <c r="G8" s="137"/>
       <c r="H8" s="23"/>
-      <c r="I8" s="82"/>
+      <c r="I8" s="79"/>
       <c r="J8" s="20"/>
       <c r="K8" s="21"/>
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
-      <c r="N8" s="83"/>
+      <c r="N8" s="80"/>
       <c r="O8" s="23"/>
-      <c r="P8" s="67"/>
+      <c r="P8" s="64"/>
       <c r="Q8" s="20"/>
       <c r="R8" s="21"/>
       <c r="S8" s="22"/>
       <c r="T8" s="22"/>
-      <c r="U8" s="68"/>
+      <c r="U8" s="65"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="140"/>
-      <c r="C9" s="95" t="s">
+      <c r="B9" s="134"/>
+      <c r="C9" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="97" t="s">
+      <c r="F9" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="141"/>
+      <c r="G9" s="135"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="100" t="s">
+      <c r="I9" s="77"/>
+      <c r="J9" s="96" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="101" t="s">
+      <c r="K9" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="102" t="s">
+      <c r="L9" s="98" t="s">
         <v>62</v>
       </c>
-      <c r="M9" s="102" t="s">
+      <c r="M9" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="N9" s="81"/>
+      <c r="N9" s="78"/>
       <c r="O9" s="14"/>
-      <c r="P9" s="66"/>
-      <c r="Q9" s="115" t="s">
+      <c r="P9" s="63"/>
+      <c r="Q9" s="110" t="s">
         <v>59</v>
       </c>
-      <c r="R9" s="116" t="s">
+      <c r="R9" s="111" t="s">
         <v>41</v>
       </c>
-      <c r="S9" s="117" t="s">
+      <c r="S9" s="112" t="s">
         <v>62</v>
       </c>
-      <c r="T9" s="117" t="s">
+      <c r="T9" s="112" t="s">
         <v>43</v>
       </c>
-      <c r="U9" s="65"/>
+      <c r="U9" s="62"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="144" t="s">
+      <c r="B10" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="28">
         <v>0.5</v>
       </c>
-      <c r="D10" s="30" t="e">
+      <c r="D10" s="29" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E10" s="31" t="e">
+      <c r="E10" s="30" t="e">
         <f>comissao/(1+C10)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F10" s="31" t="e">
+      <c r="F10" s="30" t="e">
         <f>E10/D10</f>
         <v>#NAME?</v>
       </c>
-      <c r="G10" s="141"/>
+      <c r="G10" s="135"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="84" t="s">
+      <c r="I10" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="41">
+      <c r="J10" s="39">
         <v>0.5</v>
       </c>
-      <c r="K10" s="42" t="e">
+      <c r="K10" s="40" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L10" s="43" t="e">
+      <c r="L10" s="41" t="e">
         <f>comissao/(1+J10)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M10" s="43" t="e">
+      <c r="M10" s="41" t="e">
         <f>L10/K10</f>
         <v>#NAME?</v>
       </c>
-      <c r="N10" s="81"/>
+      <c r="N10" s="78"/>
       <c r="O10" s="14"/>
-      <c r="P10" s="69" t="s">
+      <c r="P10" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="Q10" s="53">
+      <c r="Q10" s="50">
         <v>0.5</v>
       </c>
-      <c r="R10" s="54" t="e">
+      <c r="R10" s="51" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S10" s="55" t="e">
+      <c r="S10" s="52" t="e">
         <f>comissao/(Q10+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T10" s="55" t="e">
+      <c r="T10" s="52" t="e">
         <f>S10/R10</f>
         <v>#NAME?</v>
       </c>
-      <c r="U10" s="65"/>
+      <c r="U10" s="62"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="145" t="s">
+      <c r="B11" s="139" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="88">
+      <c r="C11" s="85">
         <v>0.8</v>
       </c>
-      <c r="D11" s="89" t="e">
+      <c r="D11" s="86" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E11" s="90" t="e">
+      <c r="E11" s="87" t="e">
         <f>comissao/(1+C11)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F11" s="90" t="e">
+      <c r="F11" s="87" t="e">
         <f t="shared" ref="F11:F13" si="0">E11/D11</f>
         <v>#NAME?</v>
       </c>
-      <c r="G11" s="141"/>
+      <c r="G11" s="135"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="103" t="s">
+      <c r="I11" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="104">
+      <c r="J11" s="100">
         <v>0.8</v>
       </c>
-      <c r="K11" s="105" t="e">
+      <c r="K11" s="101" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L11" s="106" t="e">
+      <c r="L11" s="102" t="e">
         <f>comissao/(1+J11)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M11" s="106" t="e">
+      <c r="M11" s="102" t="e">
         <f t="shared" ref="M11:M13" si="1">L11/K11</f>
         <v>#NAME?</v>
       </c>
-      <c r="N11" s="81"/>
+      <c r="N11" s="78"/>
       <c r="O11" s="14"/>
-      <c r="P11" s="118" t="s">
+      <c r="P11" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="Q11" s="119">
+      <c r="Q11" s="114">
         <v>0.8</v>
       </c>
-      <c r="R11" s="120" t="e">
+      <c r="R11" s="115" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S11" s="121" t="e">
+      <c r="S11" s="116" t="e">
         <f>comissao/(Q11+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T11" s="121" t="e">
+      <c r="T11" s="116" t="e">
         <f t="shared" ref="T11:T13" si="2">S11/R11</f>
         <v>#NAME?</v>
       </c>
-      <c r="U11" s="65"/>
+      <c r="U11" s="62"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="146" t="s">
+      <c r="B12" s="140" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="31">
         <v>1</v>
       </c>
-      <c r="D12" s="33" t="e">
+      <c r="D12" s="32" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E12" s="34" t="e">
+      <c r="E12" s="33" t="e">
         <f>comissao/(1+C12)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F12" s="34" t="e">
+      <c r="F12" s="33" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="G12" s="141"/>
+      <c r="G12" s="135"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="85" t="s">
+      <c r="I12" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="44">
+      <c r="J12" s="42">
         <v>1</v>
       </c>
-      <c r="K12" s="45" t="e">
+      <c r="K12" s="43" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L12" s="46" t="e">
+      <c r="L12" s="44" t="e">
         <f>comissao/(1+J12)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M12" s="46" t="e">
+      <c r="M12" s="44" t="e">
         <f t="shared" si="1"/>
         <v>#NAME?</v>
       </c>
-      <c r="N12" s="81"/>
+      <c r="N12" s="78"/>
       <c r="O12" s="14"/>
-      <c r="P12" s="70" t="s">
+      <c r="P12" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="Q12" s="56">
+      <c r="Q12" s="53">
         <v>1</v>
       </c>
-      <c r="R12" s="54" t="e">
+      <c r="R12" s="51" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S12" s="55" t="e">
+      <c r="S12" s="52" t="e">
         <f>comissao/(Q12+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T12" s="55" t="e">
+      <c r="T12" s="52" t="e">
         <f t="shared" si="2"/>
         <v>#NAME?</v>
       </c>
-      <c r="U12" s="65"/>
+      <c r="U12" s="62"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="145" t="s">
+      <c r="B13" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="88">
+      <c r="C13" s="85">
         <v>1.2</v>
       </c>
-      <c r="D13" s="89" t="e">
+      <c r="D13" s="86" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E13" s="90" t="e">
+      <c r="E13" s="87" t="e">
         <f>comissao/(1+C13)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F13" s="90" t="e">
+      <c r="F13" s="87" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="G13" s="141"/>
+      <c r="G13" s="135"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="103" t="s">
+      <c r="I13" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="104">
+      <c r="J13" s="100">
         <v>1.2</v>
       </c>
-      <c r="K13" s="105" t="e">
+      <c r="K13" s="101" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L13" s="106" t="e">
+      <c r="L13" s="102" t="e">
         <f>comissao/(1+J13)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M13" s="106" t="e">
+      <c r="M13" s="102" t="e">
         <f t="shared" si="1"/>
         <v>#NAME?</v>
       </c>
-      <c r="N13" s="81"/>
+      <c r="N13" s="78"/>
       <c r="O13" s="14"/>
-      <c r="P13" s="118" t="s">
+      <c r="P13" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="119">
+      <c r="Q13" s="114">
         <v>1.2</v>
       </c>
-      <c r="R13" s="120" t="e">
+      <c r="R13" s="115" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S13" s="121" t="e">
+      <c r="S13" s="116" t="e">
         <f>comissao/(Q13+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T13" s="121" t="e">
+      <c r="T13" s="116" t="e">
         <f t="shared" si="2"/>
         <v>#NAME?</v>
       </c>
-      <c r="U13" s="65"/>
+      <c r="U13" s="62"/>
     </row>
     <row r="14" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
-      <c r="B14" s="147"/>
+      <c r="B14" s="141"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
-      <c r="G14" s="143"/>
+      <c r="G14" s="137"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="86"/>
+      <c r="I14" s="83"/>
       <c r="J14" s="23"/>
       <c r="K14" s="23"/>
       <c r="L14" s="23"/>
       <c r="M14" s="23"/>
-      <c r="N14" s="83"/>
+      <c r="N14" s="80"/>
       <c r="O14" s="14"/>
-      <c r="P14" s="71"/>
+      <c r="P14" s="68"/>
       <c r="Q14" s="23"/>
       <c r="R14" s="23"/>
       <c r="S14" s="23"/>
       <c r="T14" s="23"/>
-      <c r="U14" s="68"/>
+      <c r="U14" s="65"/>
     </row>
     <row r="15" spans="1:21" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="61" t="s">
+      <c r="A15" s="58" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="147"/>
+      <c r="B15" s="141"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
-      <c r="G15" s="143"/>
+      <c r="G15" s="137"/>
       <c r="H15" s="14"/>
-      <c r="I15" s="86"/>
+      <c r="I15" s="83"/>
       <c r="J15" s="23"/>
       <c r="K15" s="23"/>
       <c r="L15" s="23"/>
       <c r="M15" s="23"/>
-      <c r="N15" s="83"/>
+      <c r="N15" s="80"/>
       <c r="O15" s="14"/>
-      <c r="P15" s="71"/>
+      <c r="P15" s="68"/>
       <c r="Q15" s="23"/>
       <c r="R15" s="23"/>
       <c r="S15" s="23"/>
       <c r="T15" s="23"/>
-      <c r="U15" s="68"/>
+      <c r="U15" s="65"/>
     </row>
     <row r="16" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
-      <c r="B16" s="147"/>
+      <c r="B16" s="141"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
-      <c r="G16" s="143"/>
+      <c r="G16" s="137"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="86"/>
+      <c r="I16" s="83"/>
       <c r="J16" s="23"/>
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23"/>
-      <c r="N16" s="83"/>
+      <c r="N16" s="80"/>
       <c r="O16" s="14"/>
-      <c r="P16" s="71"/>
+      <c r="P16" s="68"/>
       <c r="Q16" s="23"/>
       <c r="R16" s="23"/>
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
-      <c r="U16" s="68"/>
+      <c r="U16" s="65"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="145" t="s">
+      <c r="B17" s="139" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="90" t="e">
+      <c r="C17" s="87" t="e">
         <f>IF(Vendas = 0, E5, Métricas!Geral5/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="141"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="135"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="103" t="s">
+      <c r="I17" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="106" t="e">
+      <c r="J17" s="102" t="e">
         <f>IFERROR(SUM(Métricas!Primeiro_7dias5:Ultima5)/Venda_7dias,C17)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="81"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="78"/>
       <c r="O17" s="14"/>
-      <c r="P17" s="118" t="s">
+      <c r="P17" s="113" t="s">
         <v>42</v>
       </c>
-      <c r="Q17" s="122" t="e">
+      <c r="Q17" s="117" t="e">
         <f>IFERROR(SUM(Métricas!Primeiro_3dias5:Ultima5)/Venda_3dias,C17)</f>
         <v>#NAME?</v>
       </c>
-      <c r="R17" s="52"/>
-      <c r="S17" s="52"/>
-      <c r="T17" s="52"/>
-      <c r="U17" s="65"/>
+      <c r="R17" s="49"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="62"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="146" t="s">
+      <c r="B18" s="140" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="34">
         <f>IFERROR(Cartoes/Vendas,0)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="141"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="135"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="85" t="s">
+      <c r="I18" s="82" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="47">
+      <c r="J18" s="45">
         <f>IFERROR(Cartao_7dias/Venda_7dias,0)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="81"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="78"/>
       <c r="O18" s="14"/>
-      <c r="P18" s="69" t="s">
+      <c r="P18" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="Q18" s="57">
+      <c r="Q18" s="54">
         <f>IFERROR(Cartao_3dias/Venda_3dias,0)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="52"/>
-      <c r="S18" s="52"/>
-      <c r="T18" s="52"/>
-      <c r="U18" s="65"/>
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="62"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="145" t="s">
+      <c r="B19" s="139" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="91">
+      <c r="C19" s="88">
         <f>IFERROR(BoletosPagos/Vendas,0)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="141"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="135"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="103" t="s">
+      <c r="I19" s="99" t="s">
         <v>49</v>
       </c>
-      <c r="J19" s="107">
+      <c r="J19" s="103">
         <f>IFERROR(BoletosPago_7dias/Venda_7dias,0)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="81"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="78"/>
       <c r="O19" s="14"/>
-      <c r="P19" s="123" t="s">
+      <c r="P19" s="118" t="s">
         <v>49</v>
       </c>
-      <c r="Q19" s="124">
+      <c r="Q19" s="119">
         <f>IFERROR(BoletosPago_3dias/Venda_3dias,0)</f>
         <v>0</v>
       </c>
-      <c r="R19" s="52"/>
-      <c r="S19" s="52"/>
-      <c r="T19" s="52"/>
-      <c r="U19" s="65"/>
+      <c r="R19" s="49"/>
+      <c r="S19" s="49"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="62"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="146" t="s">
+      <c r="B20" s="140" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="34">
         <f>IFERROR(BoletosPagos/BoletosTotais,0)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="141"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="135"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="85" t="s">
+      <c r="I20" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="47">
+      <c r="J20" s="45">
         <f>IFERROR(Boletos_Pago_7dias/BoletosTotal_7dias,C20)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="81"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="78"/>
       <c r="O20" s="14"/>
-      <c r="P20" s="69" t="s">
+      <c r="P20" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="Q20" s="57">
+      <c r="Q20" s="54">
         <f>IFERROR(Boletos_Pago_3dias/BoletosTotal_3dias,C20)</f>
         <v>0</v>
       </c>
-      <c r="R20" s="52"/>
-      <c r="S20" s="52"/>
-      <c r="T20" s="52"/>
-      <c r="U20" s="65"/>
+      <c r="R20" s="49"/>
+      <c r="S20" s="49"/>
+      <c r="T20" s="49"/>
+      <c r="U20" s="62"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="145" t="s">
+      <c r="B21" s="139" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="94" t="e">
+      <c r="C21" s="90" t="e">
         <f>IF(((1/D5)*C18)+((1/D5)*C19*C20)= 0, 0.005, ((1/D5)*C18)+((1/D5)*C19*C20))</f>
         <v>#NAME?</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="141"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="135"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="103" t="s">
+      <c r="I21" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="108" t="e">
+      <c r="J21" s="104" t="e">
         <f>IF(IFERROR(((1/K5)*J18)+((1/K5)*J19*J20),C21)=0,C21,IFERROR(((1/K5)*J18)+((1/K5)*J19*J20),C21))</f>
         <v>#NAME?</v>
       </c>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="81"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="78"/>
       <c r="O21" s="14"/>
-      <c r="P21" s="118" t="s">
+      <c r="P21" s="113" t="s">
         <v>56</v>
       </c>
-      <c r="Q21" s="125" t="e">
+      <c r="Q21" s="120" t="e">
         <f>IF(IFERROR(((1/R5)*Q18)+((1/R5)*Q19*Q20),C21)=0,C21,IFERROR(((1/R5)*Q18)+((1/R5)*Q19*Q20),C21))</f>
         <v>#NAME?</v>
       </c>
-      <c r="R21" s="52"/>
-      <c r="S21" s="52"/>
-      <c r="T21" s="52"/>
-      <c r="U21" s="65"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="49"/>
+      <c r="T21" s="49"/>
+      <c r="U21" s="62"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="146" t="s">
+      <c r="B22" s="140" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="35" t="e">
+      <c r="C22" s="34" t="e">
         <f>AVERAGE(Métricas!Primeira6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="141"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="135"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="85" t="s">
+      <c r="I22" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="47" t="e">
+      <c r="J22" s="45" t="e">
         <f>AVERAGE(Métricas!Primeiro_7dias6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="81"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="78"/>
       <c r="O22" s="14"/>
-      <c r="P22" s="69" t="s">
+      <c r="P22" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="Q22" s="57" t="e">
+      <c r="Q22" s="54" t="e">
         <f>AVERAGE(Métricas!Primeiro_3dias6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
-      <c r="R22" s="52"/>
-      <c r="S22" s="52"/>
-      <c r="T22" s="52"/>
-      <c r="U22" s="65"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="49"/>
+      <c r="U22" s="62"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="138"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="141"/>
+      <c r="B23" s="132"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="135"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="81"/>
+      <c r="I23" s="75"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="78"/>
       <c r="O23" s="14"/>
-      <c r="P23" s="64"/>
-      <c r="Q23" s="52"/>
-      <c r="R23" s="52"/>
-      <c r="S23" s="52"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="65"/>
+      <c r="P23" s="61"/>
+      <c r="Q23" s="49"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="49"/>
+      <c r="U23" s="62"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="138"/>
-      <c r="C24" s="36" t="s">
+      <c r="B24" s="132"/>
+      <c r="C24" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="141"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="135"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="48" t="s">
+      <c r="I24" s="75"/>
+      <c r="J24" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="40"/>
-      <c r="N24" s="81"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="78"/>
       <c r="O24" s="14"/>
-      <c r="P24" s="64"/>
-      <c r="Q24" s="58" t="s">
+      <c r="P24" s="61"/>
+      <c r="Q24" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="R24" s="52"/>
-      <c r="S24" s="52"/>
-      <c r="T24" s="52"/>
-      <c r="U24" s="65"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="49"/>
+      <c r="U24" s="62"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="145" t="s">
+      <c r="B25" s="139" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="92" t="e">
+      <c r="C25" s="169" t="e">
         <f>(comissao/C17)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="D25" s="93">
+      <c r="D25" s="89">
         <v>0.5</v>
       </c>
-      <c r="E25" s="93">
+      <c r="E25" s="89">
         <v>0.8</v>
       </c>
-      <c r="F25" s="93">
+      <c r="F25" s="89">
         <v>1</v>
       </c>
-      <c r="G25" s="148">
+      <c r="G25" s="142">
         <v>1.2</v>
       </c>
       <c r="H25" s="14"/>
-      <c r="I25" s="103" t="s">
+      <c r="I25" s="99" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="109">
+      <c r="J25" s="168">
         <f>IFERROR((comissao/J17)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="K25" s="110">
+      <c r="K25" s="105">
         <v>0.5</v>
       </c>
-      <c r="L25" s="110">
+      <c r="L25" s="105">
         <v>0.8</v>
       </c>
-      <c r="M25" s="110">
+      <c r="M25" s="105">
         <v>1</v>
       </c>
-      <c r="N25" s="111">
+      <c r="N25" s="106">
         <v>1.2</v>
       </c>
       <c r="O25" s="14"/>
-      <c r="P25" s="118" t="s">
+      <c r="P25" s="113" t="s">
         <v>40</v>
       </c>
-      <c r="Q25" s="126">
+      <c r="Q25" s="167">
         <f>IFERROR((comissao/Q17)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="R25" s="127">
+      <c r="R25" s="121">
         <v>0.5</v>
       </c>
-      <c r="S25" s="127">
+      <c r="S25" s="121">
         <v>0.8</v>
       </c>
-      <c r="T25" s="127">
+      <c r="T25" s="121">
         <v>1</v>
       </c>
-      <c r="U25" s="128">
+      <c r="U25" s="122">
         <v>1.2</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="146" t="s">
+      <c r="B26" s="140" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="34" t="e">
+      <c r="C26" s="33" t="e">
         <f>C17</f>
         <v>#NAME?</v>
       </c>
-      <c r="D26" s="34" t="e">
+      <c r="D26" s="33" t="e">
         <f>comissao/(D25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E26" s="34" t="e">
+      <c r="E26" s="33" t="e">
         <f>comissao/(E25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F26" s="34" t="e">
+      <c r="F26" s="33" t="e">
         <f>comissao/(F25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="G26" s="149" t="e">
+      <c r="G26" s="143" t="e">
         <f>comissao/(G25+1)</f>
         <v>#NAME?</v>
       </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="85" t="s">
+      <c r="I26" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="J26" s="46" t="e">
+      <c r="J26" s="44" t="e">
         <f>J17</f>
         <v>#NAME?</v>
       </c>
-      <c r="K26" s="46" t="e">
+      <c r="K26" s="44" t="e">
         <f>comissao/(K25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L26" s="46" t="e">
+      <c r="L26" s="44" t="e">
         <f>comissao/(L25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M26" s="46" t="e">
+      <c r="M26" s="44" t="e">
         <f>comissao/(M25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N26" s="87" t="e">
+      <c r="N26" s="84" t="e">
         <f>comissao/(N25+1)</f>
         <v>#NAME?</v>
       </c>
       <c r="O26" s="14"/>
-      <c r="P26" s="69" t="s">
+      <c r="P26" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="Q26" s="55" t="e">
+      <c r="Q26" s="52" t="e">
         <f>Q17</f>
         <v>#NAME?</v>
       </c>
-      <c r="R26" s="55" t="e">
+      <c r="R26" s="52" t="e">
         <f>comissao/(R25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S26" s="55" t="e">
+      <c r="S26" s="52" t="e">
         <f>comissao/(S25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T26" s="55" t="e">
+      <c r="T26" s="52" t="e">
         <f>comissao/(T25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="U26" s="72" t="e">
+      <c r="U26" s="69" t="e">
         <f>comissao/(U25+1)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="145" t="s">
+      <c r="B27" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="89" t="e">
+      <c r="C27" s="86" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
-      <c r="D27" s="89" t="e">
+      <c r="D27" s="86" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
-      <c r="E27" s="89" t="e">
+      <c r="E27" s="86" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
-      <c r="F27" s="89" t="e">
+      <c r="F27" s="86" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
-      <c r="G27" s="150" t="e">
+      <c r="G27" s="144" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
       <c r="H27" s="14"/>
-      <c r="I27" s="103" t="s">
+      <c r="I27" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="J27" s="105" t="e">
+      <c r="J27" s="101" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
-      <c r="K27" s="105" t="e">
+      <c r="K27" s="101" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
-      <c r="L27" s="105" t="e">
+      <c r="L27" s="101" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
-      <c r="M27" s="105" t="e">
+      <c r="M27" s="101" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
-      <c r="N27" s="112" t="e">
+      <c r="N27" s="107" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
       <c r="O27" s="14"/>
-      <c r="P27" s="118" t="s">
+      <c r="P27" s="113" t="s">
         <v>41</v>
       </c>
-      <c r="Q27" s="120" t="e">
+      <c r="Q27" s="115" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
-      <c r="R27" s="120" t="e">
+      <c r="R27" s="115" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
-      <c r="S27" s="120" t="e">
+      <c r="S27" s="115" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
-      <c r="T27" s="120" t="e">
+      <c r="T27" s="115" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
-      <c r="U27" s="129" t="e">
+      <c r="U27" s="123" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="146" t="s">
+      <c r="B28" s="140" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="34" t="e">
+      <c r="C28" s="33" t="e">
         <f>C26/C27</f>
         <v>#NAME?</v>
       </c>
-      <c r="D28" s="34" t="e">
+      <c r="D28" s="33" t="e">
         <f>D26/D27</f>
         <v>#NAME?</v>
       </c>
-      <c r="E28" s="34" t="e">
+      <c r="E28" s="33" t="e">
         <f>E26/E27</f>
         <v>#NAME?</v>
       </c>
-      <c r="F28" s="34" t="e">
+      <c r="F28" s="33" t="e">
         <f>F26/F27</f>
         <v>#NAME?</v>
       </c>
-      <c r="G28" s="149" t="e">
+      <c r="G28" s="143" t="e">
         <f>G26/G27</f>
         <v>#NAME?</v>
       </c>
       <c r="H28" s="14"/>
-      <c r="I28" s="85" t="s">
+      <c r="I28" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="J28" s="46" t="e">
+      <c r="J28" s="44" t="e">
         <f>J26/J27</f>
         <v>#NAME?</v>
       </c>
-      <c r="K28" s="46" t="e">
+      <c r="K28" s="44" t="e">
         <f t="shared" ref="K28:N28" si="3">K26/K27</f>
         <v>#NAME?</v>
       </c>
-      <c r="L28" s="46" t="e">
+      <c r="L28" s="44" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
-      <c r="M28" s="46" t="e">
+      <c r="M28" s="44" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
-      <c r="N28" s="87" t="e">
+      <c r="N28" s="84" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="O28" s="14"/>
-      <c r="P28" s="69" t="s">
+      <c r="P28" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="Q28" s="55" t="e">
+      <c r="Q28" s="52" t="e">
         <f>Q26/Q27</f>
         <v>#NAME?</v>
       </c>
-      <c r="R28" s="55" t="e">
+      <c r="R28" s="52" t="e">
         <f t="shared" ref="R28:U28" si="4">R26/R27</f>
         <v>#NAME?</v>
       </c>
-      <c r="S28" s="55" t="e">
+      <c r="S28" s="52" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
-      <c r="T28" s="55" t="e">
+      <c r="T28" s="52" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
-      <c r="U28" s="72" t="e">
+      <c r="U28" s="69" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="154" t="s">
+      <c r="B29" s="148" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="155" t="e">
+      <c r="C29" s="149" t="e">
         <f>(1/C22)*C28</f>
         <v>#NAME?</v>
       </c>
-      <c r="D29" s="155" t="e">
+      <c r="D29" s="149" t="e">
         <f>(1/C22)*D28</f>
         <v>#NAME?</v>
       </c>
-      <c r="E29" s="155" t="e">
+      <c r="E29" s="149" t="e">
         <f>(1/C22)*E28</f>
         <v>#NAME?</v>
       </c>
-      <c r="F29" s="155" t="e">
+      <c r="F29" s="149" t="e">
         <f>(1/C22)*F28</f>
         <v>#NAME?</v>
       </c>
-      <c r="G29" s="156" t="e">
+      <c r="G29" s="150" t="e">
         <f>(1/C22)*G28</f>
         <v>#NAME?</v>
       </c>
       <c r="H29" s="14"/>
-      <c r="I29" s="160" t="s">
+      <c r="I29" s="154" t="s">
         <v>53</v>
       </c>
-      <c r="J29" s="161" t="e">
+      <c r="J29" s="155" t="e">
         <f>(1/J22)*J28</f>
         <v>#NAME?</v>
       </c>
-      <c r="K29" s="161" t="e">
+      <c r="K29" s="155" t="e">
         <f>(1/J22)*K28</f>
         <v>#NAME?</v>
       </c>
-      <c r="L29" s="161" t="e">
+      <c r="L29" s="155" t="e">
         <f>(1/J22)*L28</f>
         <v>#NAME?</v>
       </c>
-      <c r="M29" s="161" t="e">
+      <c r="M29" s="155" t="e">
         <f>(1/J22)*M28</f>
         <v>#NAME?</v>
       </c>
-      <c r="N29" s="162" t="e">
+      <c r="N29" s="156" t="e">
         <f>(1/J22)*N28</f>
         <v>#NAME?</v>
       </c>
       <c r="O29" s="14"/>
-      <c r="P29" s="167" t="s">
+      <c r="P29" s="161" t="s">
         <v>53</v>
       </c>
-      <c r="Q29" s="168" t="e">
+      <c r="Q29" s="162" t="e">
         <f>(1/Q22)*Q28</f>
         <v>#NAME?</v>
       </c>
-      <c r="R29" s="168" t="e">
+      <c r="R29" s="162" t="e">
         <f>(1/Q22)*R28</f>
         <v>#NAME?</v>
       </c>
-      <c r="S29" s="168" t="e">
+      <c r="S29" s="162" t="e">
         <f>(1/Q22)*S28</f>
         <v>#NAME?</v>
       </c>
-      <c r="T29" s="168" t="e">
+      <c r="T29" s="162" t="e">
         <f>(1/Q22)*T28</f>
         <v>#NAME?</v>
       </c>
-      <c r="U29" s="169" t="e">
+      <c r="U29" s="163" t="e">
         <f>(1/Q22/100)*U28</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="151"/>
-      <c r="C30" s="152"/>
-      <c r="D30" s="152"/>
-      <c r="E30" s="152"/>
-      <c r="F30" s="152"/>
-      <c r="G30" s="153"/>
+      <c r="B30" s="145"/>
+      <c r="C30" s="146"/>
+      <c r="D30" s="146"/>
+      <c r="E30" s="146"/>
+      <c r="F30" s="146"/>
+      <c r="G30" s="147"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="157"/>
-      <c r="J30" s="158"/>
-      <c r="K30" s="158"/>
-      <c r="L30" s="158"/>
-      <c r="M30" s="158"/>
-      <c r="N30" s="159"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="152"/>
+      <c r="K30" s="152"/>
+      <c r="L30" s="152"/>
+      <c r="M30" s="152"/>
+      <c r="N30" s="153"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="164"/>
-      <c r="Q30" s="165"/>
-      <c r="R30" s="165"/>
-      <c r="S30" s="165"/>
-      <c r="T30" s="165"/>
-      <c r="U30" s="166"/>
+      <c r="P30" s="158"/>
+      <c r="Q30" s="159"/>
+      <c r="R30" s="159"/>
+      <c r="S30" s="159"/>
+      <c r="T30" s="159"/>
+      <c r="U30" s="160"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
@@ -3223,10 +3241,10 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="130" t="s">
+      <c r="B34" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="131" t="s">
+      <c r="C34" s="125" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="2"/>
@@ -3277,10 +3295,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="130" t="s">
+      <c r="B36" s="124" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="132" t="s">
+      <c r="C36" s="126" t="s">
         <v>67</v>
       </c>
       <c r="D36" s="2"/>
@@ -3331,10 +3349,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="130" t="s">
+      <c r="B38" s="124" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="132" t="e">
+      <c r="C38" s="126" t="e">
         <f>IF(((1/C40)*C35)+((1/C40)*C36*C37)= 0, 0.005, ((1/C40)*C35)+((1/C40)*C36*C37))</f>
         <v>#VALUE!</v>
       </c>
@@ -3386,10 +3404,10 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="130" t="s">
+      <c r="B40" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="133" t="s">
+      <c r="C40" s="127" t="s">
         <v>74</v>
       </c>
       <c r="D40" s="2"/>
@@ -3440,10 +3458,10 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="B42" s="130" t="s">
+      <c r="B42" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="131" t="s">
+      <c r="C42" s="125" t="s">
         <v>72</v>
       </c>
       <c r="D42" s="2"/>
@@ -3494,10 +3512,10 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="130" t="s">
+      <c r="B44" s="124" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="131" t="s">
+      <c r="C44" s="125" t="s">
         <v>76</v>
       </c>
       <c r="D44" s="2"/>
@@ -3543,6 +3561,14 @@
       <c r="U45" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C5 J5 Q5 Q25 J25 C25">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- New layout to simplify use
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
   <si>
     <t>Dia:</t>
   </si>
@@ -283,6 +283,21 @@
   </si>
   <si>
     <t>Metas de ROI</t>
+  </si>
+  <si>
+    <t>Meta1</t>
+  </si>
+  <si>
+    <t>Meta2</t>
+  </si>
+  <si>
+    <t>Meta3</t>
+  </si>
+  <si>
+    <t>Maeta4</t>
+  </si>
+  <si>
+    <t>Meta4</t>
   </si>
 </sst>
 </file>
@@ -1673,11 +1688,11 @@
       <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.83203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="25.796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.796875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -1891,15 +1906,18 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C25" activeCellId="5" sqref="C5 J5 Q5 Q25 J25 C25"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="11"/>
+    <col min="9" max="9" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="11"/>
+    <col min="16" max="16" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
@@ -2194,8 +2212,8 @@
       <c r="B10" s="138" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="28">
-        <v>0.5</v>
+      <c r="C10" s="28" t="s">
+        <v>85</v>
       </c>
       <c r="D10" s="29" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
@@ -2214,8 +2232,8 @@
       <c r="I10" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="39">
-        <v>0.5</v>
+      <c r="J10" s="39" t="s">
+        <v>85</v>
       </c>
       <c r="K10" s="40" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
@@ -2234,8 +2252,8 @@
       <c r="P10" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="Q10" s="50">
-        <v>0.5</v>
+      <c r="Q10" s="50" t="s">
+        <v>85</v>
       </c>
       <c r="R10" s="51" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
@@ -2256,8 +2274,8 @@
       <c r="B11" s="139" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="85">
-        <v>0.8</v>
+      <c r="C11" s="85" t="s">
+        <v>86</v>
       </c>
       <c r="D11" s="86" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
@@ -2276,8 +2294,8 @@
       <c r="I11" s="99" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="100">
-        <v>0.8</v>
+      <c r="J11" s="100" t="s">
+        <v>86</v>
       </c>
       <c r="K11" s="101" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
@@ -2296,8 +2314,8 @@
       <c r="P11" s="113" t="s">
         <v>46</v>
       </c>
-      <c r="Q11" s="114">
-        <v>0.8</v>
+      <c r="Q11" s="114" t="s">
+        <v>86</v>
       </c>
       <c r="R11" s="115" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
@@ -2318,8 +2336,8 @@
       <c r="B12" s="140" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="31">
-        <v>1</v>
+      <c r="C12" s="31" t="s">
+        <v>87</v>
       </c>
       <c r="D12" s="32" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
@@ -2338,8 +2356,8 @@
       <c r="I12" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="42">
-        <v>1</v>
+      <c r="J12" s="42" t="s">
+        <v>87</v>
       </c>
       <c r="K12" s="43" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
@@ -2358,8 +2376,8 @@
       <c r="P12" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="Q12" s="53">
-        <v>1</v>
+      <c r="Q12" s="53" t="s">
+        <v>87</v>
       </c>
       <c r="R12" s="51" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
@@ -2380,8 +2398,8 @@
       <c r="B13" s="139" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="85">
-        <v>1.2</v>
+      <c r="C13" s="85" t="s">
+        <v>88</v>
       </c>
       <c r="D13" s="86" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
@@ -2400,8 +2418,8 @@
       <c r="I13" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="100">
-        <v>1.2</v>
+      <c r="J13" s="100" t="s">
+        <v>89</v>
       </c>
       <c r="K13" s="101" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
@@ -2420,8 +2438,8 @@
       <c r="P13" s="113" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="114">
-        <v>1.2</v>
+      <c r="Q13" s="114" t="s">
+        <v>89</v>
       </c>
       <c r="R13" s="115" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
@@ -2797,17 +2815,17 @@
         <f>(comissao/C17)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="D25" s="89">
-        <v>0.5</v>
-      </c>
-      <c r="E25" s="89">
-        <v>0.8</v>
-      </c>
-      <c r="F25" s="89">
-        <v>1</v>
-      </c>
-      <c r="G25" s="142">
-        <v>1.2</v>
+      <c r="D25" s="89" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="142" t="s">
+        <v>89</v>
       </c>
       <c r="H25" s="14"/>
       <c r="I25" s="99" t="s">
@@ -2817,17 +2835,17 @@
         <f>IFERROR((comissao/J17)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="K25" s="105">
-        <v>0.5</v>
-      </c>
-      <c r="L25" s="105">
-        <v>0.8</v>
-      </c>
-      <c r="M25" s="105">
-        <v>1</v>
-      </c>
-      <c r="N25" s="106">
-        <v>1.2</v>
+      <c r="K25" s="105" t="s">
+        <v>85</v>
+      </c>
+      <c r="L25" s="105" t="s">
+        <v>86</v>
+      </c>
+      <c r="M25" s="105" t="s">
+        <v>87</v>
+      </c>
+      <c r="N25" s="106" t="s">
+        <v>89</v>
       </c>
       <c r="O25" s="14"/>
       <c r="P25" s="113" t="s">
@@ -2837,17 +2855,17 @@
         <f>IFERROR((comissao/Q17)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="R25" s="121">
-        <v>0.5</v>
-      </c>
-      <c r="S25" s="121">
-        <v>0.8</v>
-      </c>
-      <c r="T25" s="121">
-        <v>1</v>
-      </c>
-      <c r="U25" s="122">
-        <v>1.2</v>
+      <c r="R25" s="121" t="s">
+        <v>85</v>
+      </c>
+      <c r="S25" s="121" t="s">
+        <v>86</v>
+      </c>
+      <c r="T25" s="121" t="s">
+        <v>87</v>
+      </c>
+      <c r="U25" s="122" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
- New Excel Build (updating to PhpSpreadsheet) - Error handling getting data from FB
</commit_message>
<xml_diff>
--- a/template/Template.xlsx
+++ b/template/Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="89">
   <si>
     <t>Dia:</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t>Meta3</t>
-  </si>
-  <si>
-    <t>Maeta4</t>
   </si>
   <si>
     <t>Meta4</t>
@@ -1133,7 +1130,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1151,14 +1148,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1194,7 +1189,6 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1342,7 +1336,6 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="14" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="14" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="11" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="2" fillId="14" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1354,6 +1347,22 @@
     <xf numFmtId="10" fontId="2" fillId="12" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1363,19 +1372,19 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1688,11 +1697,11 @@
       <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="25.796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.796875" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="8.796875" style="2"/>
+    <col min="1" max="1" width="25.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
@@ -1906,28 +1915,31 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="11"/>
-    <col min="9" max="9" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="11"/>
-    <col min="16" max="16" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="171" t="s">
         <v>77</v>
       </c>
+      <c r="B1" s="171"/>
+      <c r="C1" s="171"/>
+      <c r="D1" s="171"/>
+      <c r="E1" s="171"/>
+      <c r="F1" s="171"/>
+      <c r="G1" s="171"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="125" t="s">
         <v>78</v>
       </c>
       <c r="C2" s="14"/>
@@ -1936,7 +1948,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
-      <c r="I2" s="71" t="s">
+      <c r="I2" s="68" t="s">
         <v>79</v>
       </c>
       <c r="J2" s="14"/>
@@ -1945,7 +1957,7 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" s="14"/>
-      <c r="P2" s="70" t="s">
+      <c r="P2" s="67" t="s">
         <v>80</v>
       </c>
       <c r="Q2" s="14"/>
@@ -1956,1236 +1968,1236 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="129"/>
-      <c r="C3" s="130"/>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="131"/>
+      <c r="B3" s="126"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="128"/>
       <c r="H3" s="14"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="73"/>
-      <c r="N3" s="74"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="71"/>
       <c r="O3" s="14"/>
-      <c r="P3" s="157"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="60"/>
+      <c r="P3" s="154"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="56"/>
+      <c r="U3" s="57"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="132"/>
-      <c r="C4" s="94" t="s">
+      <c r="B4" s="129"/>
+      <c r="C4" s="91" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="94" t="s">
+      <c r="D4" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="133"/>
+      <c r="G4" s="130"/>
       <c r="H4" s="14"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="95" t="s">
+      <c r="I4" s="72"/>
+      <c r="J4" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="95" t="s">
+      <c r="K4" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="95" t="s">
+      <c r="L4" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="M4" s="95" t="s">
+      <c r="M4" s="92" t="s">
         <v>60</v>
       </c>
-      <c r="N4" s="76"/>
+      <c r="N4" s="73"/>
       <c r="O4" s="14"/>
-      <c r="P4" s="61"/>
-      <c r="Q4" s="108" t="s">
+      <c r="P4" s="58"/>
+      <c r="Q4" s="105" t="s">
         <v>58</v>
       </c>
-      <c r="R4" s="109" t="s">
+      <c r="R4" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="108" t="s">
+      <c r="S4" s="105" t="s">
         <v>61</v>
       </c>
-      <c r="T4" s="108" t="s">
+      <c r="T4" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="U4" s="62"/>
+      <c r="U4" s="59"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
-      <c r="B5" s="134" t="s">
+      <c r="B5" s="131" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="164" t="e">
+      <c r="C5" s="166" t="e">
         <f>(comissao/E5)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="D5" s="25" t="e">
+      <c r="D5" s="23" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E5" s="26" t="e">
+      <c r="E5" s="24" t="e">
         <f>F5*D5</f>
         <v>#NAME?</v>
       </c>
-      <c r="F5" s="26" t="e">
+      <c r="F5" s="24" t="e">
         <f>AVERAGE(Métricas!Primeira7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
-      <c r="G5" s="135"/>
+      <c r="G5" s="132"/>
       <c r="H5" s="14"/>
-      <c r="I5" s="77" t="s">
+      <c r="I5" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="165" t="e">
+      <c r="J5" s="161" t="e">
         <f>(comissao/L5)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="K5" s="36" t="e">
+      <c r="K5" s="34" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L5" s="37" t="e">
+      <c r="L5" s="35" t="e">
         <f>M5*K5</f>
         <v>#NAME?</v>
       </c>
-      <c r="M5" s="37" t="e">
+      <c r="M5" s="35" t="e">
         <f>AVERAGE(Métricas!Primeiro_7dias7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N5" s="78"/>
+      <c r="N5" s="75"/>
       <c r="O5" s="14"/>
-      <c r="P5" s="63" t="s">
+      <c r="P5" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="Q5" s="166" t="e">
+      <c r="Q5" s="162" t="e">
         <f>(comissao/S5)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="R5" s="47" t="e">
+      <c r="R5" s="45" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S5" s="48" t="e">
+      <c r="S5" s="46" t="e">
         <f>T5*R5</f>
         <v>#NAME?</v>
       </c>
-      <c r="T5" s="48" t="e">
+      <c r="T5" s="46" t="e">
         <f>AVERAGE(Métricas!Primeiro_3dias7:Ultima7)</f>
         <v>#NAME?</v>
       </c>
-      <c r="U5" s="62"/>
-    </row>
-    <row r="6" spans="1:21" s="56" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="136"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="137"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="22"/>
-      <c r="M6" s="22"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="64"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="65"/>
+      <c r="U5" s="59"/>
+    </row>
+    <row r="6" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="77"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="21"/>
+      <c r="T6" s="21"/>
+      <c r="U6" s="62"/>
     </row>
     <row r="7" spans="1:21" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="167" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="136"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="137"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="79"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="80"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="21"/>
-      <c r="S7" s="22"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="65"/>
-    </row>
-    <row r="8" spans="1:21" s="56" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="57"/>
-      <c r="B8" s="136"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="137"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="79"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="80"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="64"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="21"/>
-      <c r="S8" s="22"/>
-      <c r="T8" s="22"/>
-      <c r="U8" s="65"/>
+      <c r="B7" s="167"/>
+      <c r="C7" s="167"/>
+      <c r="D7" s="167"/>
+      <c r="E7" s="167"/>
+      <c r="F7" s="167"/>
+      <c r="G7" s="167"/>
+      <c r="H7" s="167"/>
+      <c r="I7" s="167"/>
+      <c r="J7" s="167"/>
+      <c r="K7" s="167"/>
+      <c r="L7" s="167"/>
+      <c r="M7" s="167"/>
+      <c r="N7" s="167"/>
+      <c r="O7" s="167"/>
+      <c r="P7" s="167"/>
+      <c r="Q7" s="167"/>
+      <c r="R7" s="167"/>
+      <c r="S7" s="167"/>
+      <c r="T7" s="167"/>
+      <c r="U7" s="168"/>
+    </row>
+    <row r="8" spans="1:21" s="54" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="55"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="134"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="62"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
-      <c r="B9" s="134"/>
-      <c r="C9" s="91" t="s">
+      <c r="B9" s="131"/>
+      <c r="C9" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="89" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="93" t="s">
+      <c r="E9" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="93" t="s">
+      <c r="F9" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="135"/>
+      <c r="G9" s="132"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="77"/>
-      <c r="J9" s="96" t="s">
+      <c r="I9" s="74"/>
+      <c r="J9" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="K9" s="97" t="s">
+      <c r="K9" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="98" t="s">
+      <c r="L9" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="M9" s="98" t="s">
+      <c r="M9" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="N9" s="78"/>
+      <c r="N9" s="75"/>
       <c r="O9" s="14"/>
-      <c r="P9" s="63"/>
-      <c r="Q9" s="110" t="s">
+      <c r="P9" s="60"/>
+      <c r="Q9" s="107" t="s">
         <v>59</v>
       </c>
-      <c r="R9" s="111" t="s">
+      <c r="R9" s="108" t="s">
         <v>41</v>
       </c>
-      <c r="S9" s="112" t="s">
+      <c r="S9" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="T9" s="112" t="s">
+      <c r="T9" s="109" t="s">
         <v>43</v>
       </c>
-      <c r="U9" s="62"/>
+      <c r="U9" s="59"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
-      <c r="B10" s="138" t="s">
+      <c r="B10" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="29" t="e">
+      <c r="D10" s="27" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E10" s="30" t="e">
+      <c r="E10" s="28" t="e">
         <f>comissao/(1+C10)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F10" s="30" t="e">
+      <c r="F10" s="28" t="e">
         <f>E10/D10</f>
         <v>#NAME?</v>
       </c>
-      <c r="G10" s="135"/>
+      <c r="G10" s="132"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="81" t="s">
+      <c r="I10" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="40" t="e">
+      <c r="K10" s="38" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L10" s="41" t="e">
+      <c r="L10" s="39" t="e">
         <f>comissao/(1+J10)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M10" s="41" t="e">
+      <c r="M10" s="39" t="e">
         <f>L10/K10</f>
         <v>#NAME?</v>
       </c>
-      <c r="N10" s="78"/>
+      <c r="N10" s="75"/>
       <c r="O10" s="14"/>
-      <c r="P10" s="66" t="s">
+      <c r="P10" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="Q10" s="50" t="s">
+      <c r="Q10" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="R10" s="51" t="e">
+      <c r="R10" s="49" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S10" s="52" t="e">
+      <c r="S10" s="50" t="e">
         <f>comissao/(Q10+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T10" s="52" t="e">
+      <c r="T10" s="50" t="e">
         <f>S10/R10</f>
         <v>#NAME?</v>
       </c>
-      <c r="U10" s="62"/>
+      <c r="U10" s="59"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
-      <c r="B11" s="139" t="s">
+      <c r="B11" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="D11" s="86" t="e">
+      <c r="D11" s="83" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E11" s="87" t="e">
+      <c r="E11" s="84" t="e">
         <f>comissao/(1+C11)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F11" s="87" t="e">
+      <c r="F11" s="84" t="e">
         <f t="shared" ref="F11:F13" si="0">E11/D11</f>
         <v>#NAME?</v>
       </c>
-      <c r="G11" s="135"/>
+      <c r="G11" s="132"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="99" t="s">
+      <c r="I11" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="100" t="s">
+      <c r="J11" s="97" t="s">
         <v>86</v>
       </c>
-      <c r="K11" s="101" t="e">
+      <c r="K11" s="98" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L11" s="102" t="e">
+      <c r="L11" s="99" t="e">
         <f>comissao/(1+J11)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M11" s="102" t="e">
+      <c r="M11" s="99" t="e">
         <f t="shared" ref="M11:M13" si="1">L11/K11</f>
         <v>#NAME?</v>
       </c>
-      <c r="N11" s="78"/>
+      <c r="N11" s="75"/>
       <c r="O11" s="14"/>
-      <c r="P11" s="113" t="s">
+      <c r="P11" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="Q11" s="114" t="s">
+      <c r="Q11" s="111" t="s">
         <v>86</v>
       </c>
-      <c r="R11" s="115" t="e">
+      <c r="R11" s="112" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S11" s="116" t="e">
+      <c r="S11" s="113" t="e">
         <f>comissao/(Q11+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T11" s="116" t="e">
+      <c r="T11" s="113" t="e">
         <f t="shared" ref="T11:T13" si="2">S11/R11</f>
         <v>#NAME?</v>
       </c>
-      <c r="U11" s="62"/>
+      <c r="U11" s="59"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
-      <c r="B12" s="140" t="s">
+      <c r="B12" s="137" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="32" t="e">
+      <c r="D12" s="30" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E12" s="33" t="e">
+      <c r="E12" s="31" t="e">
         <f>comissao/(1+C12)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F12" s="33" t="e">
+      <c r="F12" s="31" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="G12" s="135"/>
+      <c r="G12" s="132"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="82" t="s">
+      <c r="I12" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="J12" s="42" t="s">
+      <c r="J12" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="K12" s="43" t="e">
+      <c r="K12" s="41" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L12" s="44" t="e">
+      <c r="L12" s="42" t="e">
         <f>comissao/(1+J12)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M12" s="44" t="e">
+      <c r="M12" s="42" t="e">
         <f t="shared" si="1"/>
         <v>#NAME?</v>
       </c>
-      <c r="N12" s="78"/>
+      <c r="N12" s="75"/>
       <c r="O12" s="14"/>
-      <c r="P12" s="67" t="s">
+      <c r="P12" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="Q12" s="53" t="s">
+      <c r="Q12" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="R12" s="51" t="e">
+      <c r="R12" s="49" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S12" s="52" t="e">
+      <c r="S12" s="50" t="e">
         <f>comissao/(Q12+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T12" s="52" t="e">
+      <c r="T12" s="50" t="e">
         <f t="shared" si="2"/>
         <v>#NAME?</v>
       </c>
-      <c r="U12" s="62"/>
+      <c r="U12" s="59"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
-      <c r="B13" s="139" t="s">
+      <c r="B13" s="136" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="85" t="s">
+      <c r="C13" s="82" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="86" t="e">
+      <c r="D13" s="83" t="e">
         <f>IF(Vendas = 0, IF(ViewContents &lt; 200, 200, (QUOTIENT(ViewContents,100)*100)+100), ViewContents/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E13" s="87" t="e">
+      <c r="E13" s="84" t="e">
         <f>comissao/(1+C13)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F13" s="87" t="e">
+      <c r="F13" s="84" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="G13" s="135"/>
+      <c r="G13" s="132"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="99" t="s">
+      <c r="I13" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="100" t="s">
-        <v>89</v>
-      </c>
-      <c r="K13" s="101" t="e">
+      <c r="J13" s="97" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" s="98" t="e">
         <f>IFERROR((SUM(ViewContent_7dias:Ultimo_ViewContent))/Venda_7dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L13" s="102" t="e">
+      <c r="L13" s="99" t="e">
         <f>comissao/(1+J13)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M13" s="102" t="e">
+      <c r="M13" s="99" t="e">
         <f t="shared" si="1"/>
         <v>#NAME?</v>
       </c>
-      <c r="N13" s="78"/>
+      <c r="N13" s="75"/>
       <c r="O13" s="14"/>
-      <c r="P13" s="113" t="s">
+      <c r="P13" s="110" t="s">
         <v>55</v>
       </c>
-      <c r="Q13" s="114" t="s">
-        <v>89</v>
-      </c>
-      <c r="R13" s="115" t="e">
+      <c r="Q13" s="111" t="s">
+        <v>88</v>
+      </c>
+      <c r="R13" s="112" t="e">
         <f>IFERROR((SUM(ViewContent_3dias:Ultimo_ViewContent))/Venda_3dias,D5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S13" s="116" t="e">
+      <c r="S13" s="113" t="e">
         <f>comissao/(Q13+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T13" s="116" t="e">
+      <c r="T13" s="113" t="e">
         <f t="shared" si="2"/>
         <v>#NAME?</v>
       </c>
-      <c r="U13" s="62"/>
+      <c r="U13" s="59"/>
     </row>
     <row r="14" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
-      <c r="B14" s="141"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="137"/>
+      <c r="B14" s="138"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="134"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="83"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="80"/>
+      <c r="I14" s="80"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="77"/>
       <c r="O14" s="14"/>
-      <c r="P14" s="68"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="65"/>
+      <c r="P14" s="65"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="62"/>
     </row>
     <row r="15" spans="1:21" s="13" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="169" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="137"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="83"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="80"/>
-      <c r="O15" s="14"/>
-      <c r="P15" s="68"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="65"/>
+      <c r="B15" s="169"/>
+      <c r="C15" s="169"/>
+      <c r="D15" s="169"/>
+      <c r="E15" s="169"/>
+      <c r="F15" s="169"/>
+      <c r="G15" s="169"/>
+      <c r="H15" s="169"/>
+      <c r="I15" s="169"/>
+      <c r="J15" s="169"/>
+      <c r="K15" s="169"/>
+      <c r="L15" s="169"/>
+      <c r="M15" s="169"/>
+      <c r="N15" s="169"/>
+      <c r="O15" s="169"/>
+      <c r="P15" s="169"/>
+      <c r="Q15" s="169"/>
+      <c r="R15" s="169"/>
+      <c r="S15" s="169"/>
+      <c r="T15" s="169"/>
+      <c r="U15" s="168"/>
     </row>
     <row r="16" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
-      <c r="B16" s="141"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="137"/>
+      <c r="B16" s="138"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="134"/>
       <c r="H16" s="14"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="77"/>
       <c r="O16" s="14"/>
-      <c r="P16" s="68"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
-      <c r="U16" s="65"/>
+      <c r="P16" s="65"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="62"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
-      <c r="B17" s="139" t="s">
+      <c r="B17" s="136" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="87" t="e">
+      <c r="C17" s="84" t="e">
         <f>IF(Vendas = 0, E5, Métricas!Geral5/Vendas)</f>
         <v>#NAME?</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="135"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="132"/>
       <c r="H17" s="14"/>
-      <c r="I17" s="99" t="s">
+      <c r="I17" s="96" t="s">
         <v>42</v>
       </c>
-      <c r="J17" s="102" t="e">
+      <c r="J17" s="99" t="e">
         <f>IFERROR(SUM(Métricas!Primeiro_7dias5:Ultima5)/Venda_7dias,C17)</f>
         <v>#NAME?</v>
       </c>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="78"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="75"/>
       <c r="O17" s="14"/>
-      <c r="P17" s="113" t="s">
+      <c r="P17" s="110" t="s">
         <v>42</v>
       </c>
-      <c r="Q17" s="117" t="e">
+      <c r="Q17" s="114" t="e">
         <f>IFERROR(SUM(Métricas!Primeiro_3dias5:Ultima5)/Venda_3dias,C17)</f>
         <v>#NAME?</v>
       </c>
-      <c r="R17" s="49"/>
-      <c r="S17" s="49"/>
-      <c r="T17" s="49"/>
-      <c r="U17" s="62"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47"/>
+      <c r="T17" s="47"/>
+      <c r="U17" s="59"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
-      <c r="B18" s="140" t="s">
+      <c r="B18" s="137" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="34">
+      <c r="C18" s="32">
         <f>IFERROR(Cartoes/Vendas,0)</f>
         <v>0</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="135"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="132"/>
       <c r="H18" s="14"/>
-      <c r="I18" s="82" t="s">
+      <c r="I18" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="J18" s="45">
+      <c r="J18" s="43">
         <f>IFERROR(Cartao_7dias/Venda_7dias,0)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="38"/>
-      <c r="L18" s="38"/>
-      <c r="M18" s="38"/>
-      <c r="N18" s="78"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="75"/>
       <c r="O18" s="14"/>
-      <c r="P18" s="66" t="s">
+      <c r="P18" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="Q18" s="54">
+      <c r="Q18" s="52">
         <f>IFERROR(Cartao_3dias/Venda_3dias,0)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="49"/>
-      <c r="S18" s="49"/>
-      <c r="T18" s="49"/>
-      <c r="U18" s="62"/>
+      <c r="R18" s="47"/>
+      <c r="S18" s="47"/>
+      <c r="T18" s="47"/>
+      <c r="U18" s="59"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
-      <c r="B19" s="139" t="s">
+      <c r="B19" s="136" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="88">
+      <c r="C19" s="85">
         <f>IFERROR(BoletosPagos/Vendas,0)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="135"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="132"/>
       <c r="H19" s="14"/>
-      <c r="I19" s="99" t="s">
+      <c r="I19" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="J19" s="103">
+      <c r="J19" s="100">
         <f>IFERROR(BoletosPago_7dias/Venda_7dias,0)</f>
         <v>0</v>
       </c>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="78"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
+      <c r="M19" s="36"/>
+      <c r="N19" s="75"/>
       <c r="O19" s="14"/>
-      <c r="P19" s="118" t="s">
+      <c r="P19" s="115" t="s">
         <v>49</v>
       </c>
-      <c r="Q19" s="119">
+      <c r="Q19" s="116">
         <f>IFERROR(BoletosPago_3dias/Venda_3dias,0)</f>
         <v>0</v>
       </c>
-      <c r="R19" s="49"/>
-      <c r="S19" s="49"/>
-      <c r="T19" s="49"/>
-      <c r="U19" s="62"/>
+      <c r="R19" s="47"/>
+      <c r="S19" s="47"/>
+      <c r="T19" s="47"/>
+      <c r="U19" s="59"/>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
-      <c r="B20" s="140" t="s">
+      <c r="B20" s="137" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="34">
+      <c r="C20" s="32">
         <f>IFERROR(BoletosPagos/BoletosTotais,0)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="135"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="132"/>
       <c r="H20" s="14"/>
-      <c r="I20" s="82" t="s">
+      <c r="I20" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="45">
+      <c r="J20" s="43">
         <f>IFERROR(Boletos_Pago_7dias/BoletosTotal_7dias,C20)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="38"/>
-      <c r="L20" s="38"/>
-      <c r="M20" s="38"/>
-      <c r="N20" s="78"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+      <c r="M20" s="36"/>
+      <c r="N20" s="75"/>
       <c r="O20" s="14"/>
-      <c r="P20" s="66" t="s">
+      <c r="P20" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="Q20" s="54">
+      <c r="Q20" s="52">
         <f>IFERROR(Boletos_Pago_3dias/BoletosTotal_3dias,C20)</f>
         <v>0</v>
       </c>
-      <c r="R20" s="49"/>
-      <c r="S20" s="49"/>
-      <c r="T20" s="49"/>
-      <c r="U20" s="62"/>
+      <c r="R20" s="47"/>
+      <c r="S20" s="47"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="59"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
-      <c r="B21" s="139" t="s">
+      <c r="B21" s="136" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="90" t="e">
+      <c r="C21" s="87" t="e">
         <f>IF(((1/D5)*C18)+((1/D5)*C19*C20)= 0, 0.005, ((1/D5)*C18)+((1/D5)*C19*C20))</f>
         <v>#NAME?</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="135"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="132"/>
       <c r="H21" s="14"/>
-      <c r="I21" s="99" t="s">
+      <c r="I21" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="J21" s="104" t="e">
+      <c r="J21" s="101" t="e">
         <f>IF(IFERROR(((1/K5)*J18)+((1/K5)*J19*J20),C21)=0,C21,IFERROR(((1/K5)*J18)+((1/K5)*J19*J20),C21))</f>
         <v>#NAME?</v>
       </c>
-      <c r="K21" s="38"/>
-      <c r="L21" s="38"/>
-      <c r="M21" s="38"/>
-      <c r="N21" s="78"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="75"/>
       <c r="O21" s="14"/>
-      <c r="P21" s="113" t="s">
+      <c r="P21" s="110" t="s">
         <v>56</v>
       </c>
-      <c r="Q21" s="120" t="e">
+      <c r="Q21" s="117" t="e">
         <f>IF(IFERROR(((1/R5)*Q18)+((1/R5)*Q19*Q20),C21)=0,C21,IFERROR(((1/R5)*Q18)+((1/R5)*Q19*Q20),C21))</f>
         <v>#NAME?</v>
       </c>
-      <c r="R21" s="49"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="49"/>
-      <c r="U21" s="62"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="59"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
-      <c r="B22" s="140" t="s">
+      <c r="B22" s="137" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="34" t="e">
+      <c r="C22" s="32" t="e">
         <f>AVERAGE(Métricas!Primeira6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="135"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="132"/>
       <c r="H22" s="14"/>
-      <c r="I22" s="82" t="s">
+      <c r="I22" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="45" t="e">
+      <c r="J22" s="43" t="e">
         <f>AVERAGE(Métricas!Primeiro_7dias6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
-      <c r="K22" s="38"/>
-      <c r="L22" s="38"/>
-      <c r="M22" s="38"/>
-      <c r="N22" s="78"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+      <c r="M22" s="36"/>
+      <c r="N22" s="75"/>
       <c r="O22" s="14"/>
-      <c r="P22" s="66" t="s">
+      <c r="P22" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="Q22" s="54" t="e">
+      <c r="Q22" s="52" t="e">
         <f>AVERAGE(Métricas!Primeiro_3dias6:Ultima6)/100</f>
         <v>#NAME?</v>
       </c>
-      <c r="R22" s="49"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="49"/>
-      <c r="U22" s="62"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="59"/>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
-      <c r="B23" s="132"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="135"/>
+      <c r="B23" s="129"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="132"/>
       <c r="H23" s="14"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="38"/>
-      <c r="N23" s="78"/>
+      <c r="I23" s="72"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="75"/>
       <c r="O23" s="14"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="49"/>
-      <c r="R23" s="49"/>
-      <c r="S23" s="49"/>
-      <c r="T23" s="49"/>
-      <c r="U23" s="62"/>
+      <c r="P23" s="58"/>
+      <c r="Q23" s="47"/>
+      <c r="R23" s="47"/>
+      <c r="S23" s="47"/>
+      <c r="T23" s="47"/>
+      <c r="U23" s="59"/>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="132"/>
-      <c r="C24" s="35" t="s">
+      <c r="B24" s="129"/>
+      <c r="C24" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="135"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="132"/>
       <c r="H24" s="14"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="46" t="s">
+      <c r="I24" s="72"/>
+      <c r="J24" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="K24" s="38"/>
-      <c r="L24" s="38"/>
-      <c r="M24" s="38"/>
-      <c r="N24" s="78"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="75"/>
       <c r="O24" s="14"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="55" t="s">
+      <c r="P24" s="58"/>
+      <c r="Q24" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="R24" s="49"/>
-      <c r="S24" s="49"/>
-      <c r="T24" s="49"/>
-      <c r="U24" s="62"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="47"/>
+      <c r="T24" s="47"/>
+      <c r="U24" s="59"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
-      <c r="B25" s="139" t="s">
+      <c r="B25" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="169" t="e">
+      <c r="C25" s="165" t="e">
         <f>(comissao/C17)-1</f>
         <v>#NAME?</v>
       </c>
-      <c r="D25" s="89" t="s">
+      <c r="D25" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="E25" s="89" t="s">
+      <c r="E25" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="89" t="s">
+      <c r="F25" s="86" t="s">
         <v>87</v>
       </c>
-      <c r="G25" s="142" t="s">
-        <v>89</v>
+      <c r="G25" s="139" t="s">
+        <v>88</v>
       </c>
       <c r="H25" s="14"/>
-      <c r="I25" s="99" t="s">
+      <c r="I25" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="J25" s="168">
+      <c r="J25" s="164">
         <f>IFERROR((comissao/J17)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="K25" s="105" t="s">
+      <c r="K25" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="L25" s="105" t="s">
+      <c r="L25" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="M25" s="105" t="s">
+      <c r="M25" s="102" t="s">
         <v>87</v>
       </c>
-      <c r="N25" s="106" t="s">
-        <v>89</v>
+      <c r="N25" s="103" t="s">
+        <v>88</v>
       </c>
       <c r="O25" s="14"/>
-      <c r="P25" s="113" t="s">
+      <c r="P25" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="Q25" s="167">
+      <c r="Q25" s="163">
         <f>IFERROR((comissao/Q17)-1,0)</f>
         <v>0</v>
       </c>
-      <c r="R25" s="121" t="s">
+      <c r="R25" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="S25" s="121" t="s">
+      <c r="S25" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="T25" s="121" t="s">
+      <c r="T25" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="U25" s="122" t="s">
-        <v>89</v>
+      <c r="U25" s="119" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
-      <c r="B26" s="140" t="s">
+      <c r="B26" s="137" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="33" t="e">
+      <c r="C26" s="31" t="e">
         <f>C17</f>
         <v>#NAME?</v>
       </c>
-      <c r="D26" s="33" t="e">
+      <c r="D26" s="31" t="e">
         <f>comissao/(D25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="E26" s="33" t="e">
+      <c r="E26" s="31" t="e">
         <f>comissao/(E25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="F26" s="33" t="e">
+      <c r="F26" s="31" t="e">
         <f>comissao/(F25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="G26" s="143" t="e">
+      <c r="G26" s="140" t="e">
         <f>comissao/(G25+1)</f>
         <v>#NAME?</v>
       </c>
       <c r="H26" s="14"/>
-      <c r="I26" s="82" t="s">
+      <c r="I26" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="J26" s="44" t="e">
+      <c r="J26" s="42" t="e">
         <f>J17</f>
         <v>#NAME?</v>
       </c>
-      <c r="K26" s="44" t="e">
+      <c r="K26" s="42" t="e">
         <f>comissao/(K25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="L26" s="44" t="e">
+      <c r="L26" s="42" t="e">
         <f>comissao/(L25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="M26" s="44" t="e">
+      <c r="M26" s="42" t="e">
         <f>comissao/(M25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="N26" s="84" t="e">
+      <c r="N26" s="81" t="e">
         <f>comissao/(N25+1)</f>
         <v>#NAME?</v>
       </c>
       <c r="O26" s="14"/>
-      <c r="P26" s="66" t="s">
+      <c r="P26" s="63" t="s">
         <v>42</v>
       </c>
-      <c r="Q26" s="52" t="e">
+      <c r="Q26" s="50" t="e">
         <f>Q17</f>
         <v>#NAME?</v>
       </c>
-      <c r="R26" s="52" t="e">
+      <c r="R26" s="50" t="e">
         <f>comissao/(R25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="S26" s="52" t="e">
+      <c r="S26" s="50" t="e">
         <f>comissao/(S25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="T26" s="52" t="e">
+      <c r="T26" s="50" t="e">
         <f>comissao/(T25+1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="U26" s="69" t="e">
+      <c r="U26" s="66" t="e">
         <f>comissao/(U25+1)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
-      <c r="B27" s="139" t="s">
+      <c r="B27" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="86" t="e">
+      <c r="C27" s="83" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
-      <c r="D27" s="86" t="e">
+      <c r="D27" s="83" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
-      <c r="E27" s="86" t="e">
+      <c r="E27" s="83" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
-      <c r="F27" s="86" t="e">
+      <c r="F27" s="83" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
-      <c r="G27" s="144" t="e">
+      <c r="G27" s="141" t="e">
         <f>1/C21</f>
         <v>#NAME?</v>
       </c>
       <c r="H27" s="14"/>
-      <c r="I27" s="99" t="s">
+      <c r="I27" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="J27" s="101" t="e">
+      <c r="J27" s="98" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
-      <c r="K27" s="101" t="e">
+      <c r="K27" s="98" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
-      <c r="L27" s="101" t="e">
+      <c r="L27" s="98" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
-      <c r="M27" s="101" t="e">
+      <c r="M27" s="98" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
-      <c r="N27" s="107" t="e">
+      <c r="N27" s="104" t="e">
         <f>1/J21</f>
         <v>#NAME?</v>
       </c>
       <c r="O27" s="14"/>
-      <c r="P27" s="113" t="s">
+      <c r="P27" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="Q27" s="115" t="e">
+      <c r="Q27" s="112" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
-      <c r="R27" s="115" t="e">
+      <c r="R27" s="112" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
-      <c r="S27" s="115" t="e">
+      <c r="S27" s="112" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
-      <c r="T27" s="115" t="e">
+      <c r="T27" s="112" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
-      <c r="U27" s="123" t="e">
+      <c r="U27" s="120" t="e">
         <f>1/Q21</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
-      <c r="B28" s="140" t="s">
+      <c r="B28" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="33" t="e">
+      <c r="C28" s="31" t="e">
         <f>C26/C27</f>
         <v>#NAME?</v>
       </c>
-      <c r="D28" s="33" t="e">
+      <c r="D28" s="31" t="e">
         <f>D26/D27</f>
         <v>#NAME?</v>
       </c>
-      <c r="E28" s="33" t="e">
+      <c r="E28" s="31" t="e">
         <f>E26/E27</f>
         <v>#NAME?</v>
       </c>
-      <c r="F28" s="33" t="e">
+      <c r="F28" s="31" t="e">
         <f>F26/F27</f>
         <v>#NAME?</v>
       </c>
-      <c r="G28" s="143" t="e">
+      <c r="G28" s="140" t="e">
         <f>G26/G27</f>
         <v>#NAME?</v>
       </c>
       <c r="H28" s="14"/>
-      <c r="I28" s="82" t="s">
+      <c r="I28" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="J28" s="44" t="e">
+      <c r="J28" s="42" t="e">
         <f>J26/J27</f>
         <v>#NAME?</v>
       </c>
-      <c r="K28" s="44" t="e">
+      <c r="K28" s="42" t="e">
         <f t="shared" ref="K28:N28" si="3">K26/K27</f>
         <v>#NAME?</v>
       </c>
-      <c r="L28" s="44" t="e">
+      <c r="L28" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
-      <c r="M28" s="44" t="e">
+      <c r="M28" s="42" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
-      <c r="N28" s="84" t="e">
+      <c r="N28" s="81" t="e">
         <f t="shared" si="3"/>
         <v>#NAME?</v>
       </c>
       <c r="O28" s="14"/>
-      <c r="P28" s="66" t="s">
+      <c r="P28" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="Q28" s="52" t="e">
+      <c r="Q28" s="50" t="e">
         <f>Q26/Q27</f>
         <v>#NAME?</v>
       </c>
-      <c r="R28" s="52" t="e">
+      <c r="R28" s="50" t="e">
         <f t="shared" ref="R28:U28" si="4">R26/R27</f>
         <v>#NAME?</v>
       </c>
-      <c r="S28" s="52" t="e">
+      <c r="S28" s="50" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
-      <c r="T28" s="52" t="e">
+      <c r="T28" s="50" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
-      <c r="U28" s="69" t="e">
+      <c r="U28" s="66" t="e">
         <f t="shared" si="4"/>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="2"/>
-      <c r="B29" s="148" t="s">
+      <c r="B29" s="145" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="149" t="e">
+      <c r="C29" s="146" t="e">
         <f>(1/C22)*C28</f>
         <v>#NAME?</v>
       </c>
-      <c r="D29" s="149" t="e">
+      <c r="D29" s="146" t="e">
         <f>(1/C22)*D28</f>
         <v>#NAME?</v>
       </c>
-      <c r="E29" s="149" t="e">
+      <c r="E29" s="146" t="e">
         <f>(1/C22)*E28</f>
         <v>#NAME?</v>
       </c>
-      <c r="F29" s="149" t="e">
+      <c r="F29" s="146" t="e">
         <f>(1/C22)*F28</f>
         <v>#NAME?</v>
       </c>
-      <c r="G29" s="150" t="e">
+      <c r="G29" s="147" t="e">
         <f>(1/C22)*G28</f>
         <v>#NAME?</v>
       </c>
       <c r="H29" s="14"/>
-      <c r="I29" s="154" t="s">
+      <c r="I29" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="J29" s="155" t="e">
+      <c r="J29" s="152" t="e">
         <f>(1/J22)*J28</f>
         <v>#NAME?</v>
       </c>
-      <c r="K29" s="155" t="e">
+      <c r="K29" s="152" t="e">
         <f>(1/J22)*K28</f>
         <v>#NAME?</v>
       </c>
-      <c r="L29" s="155" t="e">
+      <c r="L29" s="152" t="e">
         <f>(1/J22)*L28</f>
         <v>#NAME?</v>
       </c>
-      <c r="M29" s="155" t="e">
+      <c r="M29" s="152" t="e">
         <f>(1/J22)*M28</f>
         <v>#NAME?</v>
       </c>
-      <c r="N29" s="156" t="e">
+      <c r="N29" s="153" t="e">
         <f>(1/J22)*N28</f>
         <v>#NAME?</v>
       </c>
       <c r="O29" s="14"/>
-      <c r="P29" s="161" t="s">
+      <c r="P29" s="158" t="s">
         <v>53</v>
       </c>
-      <c r="Q29" s="162" t="e">
+      <c r="Q29" s="159" t="e">
         <f>(1/Q22)*Q28</f>
         <v>#NAME?</v>
       </c>
-      <c r="R29" s="162" t="e">
+      <c r="R29" s="159" t="e">
         <f>(1/Q22)*R28</f>
         <v>#NAME?</v>
       </c>
-      <c r="S29" s="162" t="e">
+      <c r="S29" s="159" t="e">
         <f>(1/Q22)*S28</f>
         <v>#NAME?</v>
       </c>
-      <c r="T29" s="162" t="e">
+      <c r="T29" s="159" t="e">
         <f>(1/Q22)*T28</f>
         <v>#NAME?</v>
       </c>
-      <c r="U29" s="163" t="e">
+      <c r="U29" s="160" t="e">
         <f>(1/Q22/100)*U28</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A30" s="2"/>
-      <c r="B30" s="145"/>
-      <c r="C30" s="146"/>
-      <c r="D30" s="146"/>
-      <c r="E30" s="146"/>
-      <c r="F30" s="146"/>
-      <c r="G30" s="147"/>
+      <c r="B30" s="142"/>
+      <c r="C30" s="143"/>
+      <c r="D30" s="143"/>
+      <c r="E30" s="143"/>
+      <c r="F30" s="143"/>
+      <c r="G30" s="144"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="152"/>
-      <c r="K30" s="152"/>
-      <c r="L30" s="152"/>
-      <c r="M30" s="152"/>
-      <c r="N30" s="153"/>
+      <c r="I30" s="148"/>
+      <c r="J30" s="149"/>
+      <c r="K30" s="149"/>
+      <c r="L30" s="149"/>
+      <c r="M30" s="149"/>
+      <c r="N30" s="150"/>
       <c r="O30" s="2"/>
-      <c r="P30" s="158"/>
-      <c r="Q30" s="159"/>
-      <c r="R30" s="159"/>
-      <c r="S30" s="159"/>
-      <c r="T30" s="159"/>
-      <c r="U30" s="160"/>
+      <c r="P30" s="155"/>
+      <c r="Q30" s="156"/>
+      <c r="R30" s="156"/>
+      <c r="S30" s="156"/>
+      <c r="T30" s="156"/>
+      <c r="U30" s="157"/>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
@@ -3211,12 +3223,12 @@
       <c r="U31" s="2"/>
     </row>
     <row r="32" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="170" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="B32" s="170"/>
+      <c r="C32" s="170"/>
+      <c r="D32" s="170"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -3259,10 +3271,10 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
-      <c r="B34" s="124" t="s">
+      <c r="B34" s="121" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="125" t="s">
+      <c r="C34" s="122" t="s">
         <v>66</v>
       </c>
       <c r="D34" s="2"/>
@@ -3289,7 +3301,7 @@
       <c r="B35" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="19" t="s">
+      <c r="C35" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D35" s="2"/>
@@ -3313,10 +3325,10 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A36" s="2"/>
-      <c r="B36" s="124" t="s">
+      <c r="B36" s="121" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="126" t="s">
+      <c r="C36" s="123" t="s">
         <v>67</v>
       </c>
       <c r="D36" s="2"/>
@@ -3343,7 +3355,7 @@
       <c r="B37" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="18" t="s">
         <v>69</v>
       </c>
       <c r="D37" s="2"/>
@@ -3367,10 +3379,10 @@
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A38" s="2"/>
-      <c r="B38" s="124" t="s">
+      <c r="B38" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="126" t="e">
+      <c r="C38" s="123" t="e">
         <f>IF(((1/C40)*C35)+((1/C40)*C36*C37)= 0, 0.005, ((1/C40)*C35)+((1/C40)*C36*C37))</f>
         <v>#VALUE!</v>
       </c>
@@ -3398,7 +3410,7 @@
       <c r="B39" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="17" t="s">
         <v>70</v>
       </c>
       <c r="D39" s="2"/>
@@ -3422,10 +3434,10 @@
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A40" s="2"/>
-      <c r="B40" s="124" t="s">
+      <c r="B40" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="127" t="s">
+      <c r="C40" s="124" t="s">
         <v>74</v>
       </c>
       <c r="D40" s="2"/>
@@ -3452,7 +3464,7 @@
       <c r="B41" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="17" t="s">
         <v>71</v>
       </c>
       <c r="D41" s="2"/>
@@ -3476,10 +3488,10 @@
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A42" s="2"/>
-      <c r="B42" s="124" t="s">
+      <c r="B42" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="125" t="s">
+      <c r="C42" s="122" t="s">
         <v>72</v>
       </c>
       <c r="D42" s="2"/>
@@ -3506,7 +3518,7 @@
       <c r="B43" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="17" t="s">
         <v>73</v>
       </c>
       <c r="D43" s="2"/>
@@ -3530,10 +3542,10 @@
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A44" s="2"/>
-      <c r="B44" s="124" t="s">
+      <c r="B44" s="121" t="s">
         <v>75</v>
       </c>
-      <c r="C44" s="125" t="s">
+      <c r="C44" s="122" t="s">
         <v>76</v>
       </c>
       <c r="D44" s="2"/>
@@ -3579,11 +3591,17 @@
       <c r="U45" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A7:U7"/>
+    <mergeCell ref="A15:U15"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <conditionalFormatting sqref="C5 J5 Q5 Q25 J25 C25">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>